<commit_message>
settings / access control mapping
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@53753 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="302">
   <si>
     <t>Dashboard</t>
   </si>
@@ -817,6 +817,111 @@
   </si>
   <si>
     <t>saveChangesBtn</t>
+  </si>
+  <si>
+    <t>add / edit access control profile window</t>
+  </si>
+  <si>
+    <t>acDrilldown.</t>
+  </si>
+  <si>
+    <t>profileNameTi</t>
+  </si>
+  <si>
+    <t>profile name</t>
+  </si>
+  <si>
+    <t>descriptionTa</t>
+  </si>
+  <si>
+    <t>profile description</t>
+  </si>
+  <si>
+    <t>anySiteRaddioBtn</t>
+  </si>
+  <si>
+    <t>approvedSitesRadioBtn</t>
+  </si>
+  <si>
+    <t>approvedDomainsList</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>add domain</t>
+  </si>
+  <si>
+    <t>remove domain</t>
+  </si>
+  <si>
+    <t>authorised domain list</t>
+  </si>
+  <si>
+    <t>notApprovedSitesRadioBtn</t>
+  </si>
+  <si>
+    <t>notApprovedDomainsList</t>
+  </si>
+  <si>
+    <t>unauthorised domains list</t>
+  </si>
+  <si>
+    <t>removeAuthorisedBtn</t>
+  </si>
+  <si>
+    <t>addAuthorisedBtn</t>
+  </si>
+  <si>
+    <t>addUnauthorisedBtn</t>
+  </si>
+  <si>
+    <t>removeUnauthorisedBtn</t>
+  </si>
+  <si>
+    <t>allCountriesRaddioBtn</t>
+  </si>
+  <si>
+    <t>approvedCountiesRadioBtn</t>
+  </si>
+  <si>
+    <t>approvedCountriesList</t>
+  </si>
+  <si>
+    <t>addRemoveCountriesBtn</t>
+  </si>
+  <si>
+    <t>notApprovedCountriesRadioBtn</t>
+  </si>
+  <si>
+    <t>notApprovedCountriesList</t>
+  </si>
+  <si>
+    <t>restrictCountriesLinkButton</t>
+  </si>
+  <si>
+    <t>secureKSCBBtn</t>
+  </si>
+  <si>
+    <t>secure viewing</t>
+  </si>
+  <si>
+    <t>freePerviewCBBtn</t>
+  </si>
+  <si>
+    <t>free preview</t>
+  </si>
+  <si>
+    <t>freePreviewDuration</t>
+  </si>
+  <si>
+    <t>time fir free preview</t>
+  </si>
+  <si>
+    <t>SM_TimeEntry</t>
+  </si>
+  <si>
+    <t>save changes</t>
   </si>
 </sst>
 </file>
@@ -1202,18 +1307,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G194"/>
+  <dimension ref="A1:G212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="28.625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.25" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.125" style="2" bestFit="1" customWidth="1"/>
@@ -1526,7 +1631,7 @@
         <v>account.accessControl.accessControlProfilesTable</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1541,7 +1646,7 @@
         <v>account.accessControl.addAccessControlButton</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -1556,1294 +1661,1333 @@
         <v>account.accessControl.deleteProfilesBtn</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
-        <v>45</v>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>47</v>
+        <v>269</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>CONCATENATE($C$36,C37)</f>
-        <v>account.transcodingconversionSettingsTable1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="2" t="s">
-        <v>46</v>
+        <v>acDrilldown.profileNameTi</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>48</v>
+        <v>271</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f t="shared" ref="D38:D39" si="3">CONCATENATE($C$36,C38)</f>
-        <v>account.transcodingswitchModeBtn</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
-        <v>50</v>
-      </c>
+        <f t="shared" ref="D38:D58" si="3">CONCATENATE($C$36,C38)</f>
+        <v>acDrilldown.descriptionTa</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>225</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>49</v>
+        <v>273</v>
       </c>
       <c r="D39" s="2" t="str">
         <f t="shared" si="3"/>
+        <v>acDrilldown.anySiteRaddioBtn</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D40" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.approvedSitesRadioBtn</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D41" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.approvedDomainsList</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.addAuthorisedBtn</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D43" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.removeAuthorisedBtn</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D44" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.notApprovedSitesRadioBtn</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D45" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.notApprovedDomainsList</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.addUnauthorisedBtn</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.removeUnauthorisedBtn</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D48" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.allCountriesRaddioBtn</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="B49" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.approvedCountiesRadioBtn</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.approvedCountriesList</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.addRemoveCountriesBtn</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="B52" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.notApprovedCountriesRadioBtn</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="B53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.notApprovedCountriesList</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D54" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.restrictCountriesLinkButton</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D55" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.secureKSCBBtn</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D56" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.freePerviewCBBtn</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D57" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.freePreviewDuration</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>acDrilldown.submitBtn</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="2" t="str">
+        <f>CONCATENATE($C$60,C61)</f>
+        <v>account.transcodingconversionSettingsTable1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="2" t="str">
+        <f t="shared" ref="D62:D63" si="4">CONCATENATE($C$60,C62)</f>
+        <v>account.transcodingswitchModeBtn</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>account.transcodingsaveButton</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="5" t="s">
+    <row r="66" spans="1:7">
+      <c r="A66" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="2" t="str">
-        <f>CONCATENATE($C$42,C43)</f>
-        <v>account.upgrade.customFieldsTable</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="2" t="str">
-        <f>CONCATENATE($C$42,C44)</f>
-        <v>account.upgrade.addFieldButton</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="2" t="str">
-        <f>CONCATENATE($C$42,C45)</f>
-        <v>account.upgrade.deleteCustomDataField</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="2" t="str">
-        <f>CONCATENATE($C$51,C52)</f>
-        <v>admin.users.table</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" s="2" t="str">
-        <f>CONCATENATE($C$51,C53)</f>
-        <v>admin.users.addBtn</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="2" t="str">
-        <f>CONCATENATE($C$51,C54)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="2" t="str">
-        <f>CONCATENATE($C$51,C55)</f>
-        <v>admin.users.table</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" s="2" t="str">
-        <f>CONCATENATE($C$51,C58)</f>
-        <v>admin.users.table</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D59" s="2" t="str">
-        <f>CONCATENATE($C$51,C59)</f>
-        <v>admin.users.addBtn</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" s="2" t="str">
-        <f>CONCATENATE($C$51,C60)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="2" t="str">
-        <f>CONCATENATE($C$51,C61)</f>
-        <v>admin.users.table</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="2" t="str">
-        <f>CONCATENATE($C$65,C66)</f>
-        <v>studio.playerList.templatesHolder</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>80</v>
+        <v>52</v>
+      </c>
+      <c r="D67" s="2" t="str">
+        <f>CONCATENATE($C$66,C67)</f>
+        <v>account.upgrade.customFieldsTable</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="2" t="str">
+        <f>CONCATENATE($C$66,C68)</f>
+        <v>account.upgrade.addFieldButton</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="2" t="str">
+        <f>CONCATENATE($C$66,C69)</f>
+        <v>account.upgrade.deleteCustomDataField</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" s="2" t="str">
+        <f>CONCATENATE($C$75,C76)</f>
+        <v>admin.users.table</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="2" t="str">
+        <f>CONCATENATE($C$75,C77)</f>
+        <v>admin.users.addBtn</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D78" s="2" t="str">
+        <f>CONCATENATE($C$75,C78)</f>
+        <v>admin.users.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="2" t="str">
+        <f>CONCATENATE($C$75,C79)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" s="2" t="str">
+        <f>CONCATENATE($C$75,C82)</f>
+        <v>admin.users.table</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="2" t="str">
+        <f>CONCATENATE($C$75,C83)</f>
+        <v>admin.users.addBtn</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="2" t="str">
+        <f>CONCATENATE($C$75,C84)</f>
+        <v>admin.users.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85" s="2" t="str">
+        <f>CONCATENATE($C$75,C85)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D90" s="2" t="str">
+        <f>CONCATENATE($C$89,C90)</f>
+        <v>studio.playerList.templatesHolder</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D68" s="2" t="str">
-        <f>CONCATENATE($C$67,C68)</f>
+      <c r="D92" s="2" t="str">
+        <f>CONCATENATE($C$91,C92)</f>
         <v>wizard.wizardSaveBtn</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="1" t="s">
+    <row r="93" spans="1:7">
+      <c r="A93" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="B93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D69" s="1" t="str">
-        <f t="shared" ref="D69" si="4">CONCATENATE($C$67,C69)</f>
+      <c r="D93" s="1" t="str">
+        <f t="shared" ref="D93" si="5">CONCATENATE($C$91,C93)</f>
         <v>wizard.templatePage.</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="1" t="s">
+    <row r="94" spans="1:7">
+      <c r="A94" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B94" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D70" s="1" t="str">
-        <f>CONCATENATE($D$69,C70)</f>
+      <c r="D94" s="1" t="str">
+        <f t="shared" ref="D94:D101" si="6">CONCATENATE($D$93,C94)</f>
         <v>wizard.templatePage.all</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="1" t="s">
+    <row r="95" spans="1:7">
+      <c r="A95" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D71" s="1" t="str">
-        <f>CONCATENATE($D$69,C71)</f>
+      <c r="D95" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.playerName</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="1" t="s">
+    <row r="96" spans="1:7">
+      <c r="A96" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D72" s="1" t="str">
-        <f>CONCATENATE($D$69,C72)</f>
+      <c r="D96" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.keepOriginalRatio</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="1" t="s">
+    <row r="97" spans="1:6">
+      <c r="A97" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D73" s="1" t="str">
-        <f>CONCATENATE($D$69,C73)</f>
+      <c r="D97" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.streachMediaToFitPlayer</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="1" t="s">
+    <row r="98" spans="1:6">
+      <c r="A98" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D74" s="1" t="str">
-        <f>CONCATENATE($D$69,C74)</f>
+      <c r="D98" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.templateAutoPlay</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="1" t="s">
+    <row r="99" spans="1:6">
+      <c r="A99" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D75" s="1" t="str">
-        <f>CONCATENATE($D$69,C75)</f>
+      <c r="D99" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.templateAutoMute</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="1" t="s">
+    <row r="100" spans="1:6">
+      <c r="A100" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D76" s="1" t="str">
-        <f>CONCATENATE($D$69,C76)</f>
+      <c r="D100" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.playlistAutoContinue</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="1" t="s">
+    <row r="101" spans="1:6">
+      <c r="A101" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D77" s="1" t="str">
-        <f>CONCATENATE($D$69,C77)</f>
+      <c r="D101" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>wizard.templatePage.playlistImagesInterval</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D79" s="2" t="str">
-        <f>CONCATENATE($C$67,C79)</f>
-        <v>wizard.featurePage.</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D80" s="2" t="str">
-        <f>CONCATENATE($D$79,C80)</f>
-        <v>wizard.featurePage.accordi</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D81" s="2" t="str">
-        <f>CONCATENATE($D$79,C81)</f>
-        <v>wizard.featurePage.featureScreen</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D82" s="2" t="str">
-        <f>CONCATENATE($D$79,C82)</f>
-        <v>wizard.featurePage.keyValueBox</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D84" s="2" t="str">
-        <f>CONCATENATE($C$67,C84)</f>
-        <v>wizard.advertizingPage</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D86" s="2" t="str">
-        <f>CONCATENATE($C$67,C86)</f>
-        <v>wizard.stylePage</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D88" s="2" t="str">
-        <f>CONCATENATE($C$67,C88)</f>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D89" s="2" t="str">
-        <f>CONCATENATE($D$88,C89)</f>
-        <v>wizard.contentPage.all</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="D90" s="2" t="str">
-        <f t="shared" ref="D90:D95" si="5">CONCATENATE($D$88,C90)</f>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="D91" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="D92" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="D93" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="D94" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="D95" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D97" s="2" t="str">
-        <f>CONCATENATE($C$67,C97)</f>
-        <v>wizard.previewPlayerPage.</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D98" s="2" t="str">
-        <f>CONCATENATE($D$97,C98)</f>
-        <v>wizard.previewPlayerPage.controls</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D99" s="2" t="str">
-        <f>CONCATENATE($D$97,C99)</f>
-        <v>wizard.previewPlayerPage.openClosePreview</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D100" s="2" t="str">
-        <f>CONCATENATE($D$97,C100)</f>
-        <v>wizard.previewPlayerPage.kdpWidth</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D101" s="2" t="str">
-        <f>CONCATENATE($D$97,C101)</f>
-        <v>wizard.previewPlayerPage.kdpHeight</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D102" s="2" t="str">
-        <f>CONCATENATE($D$97,C102)</f>
-        <v>wizard.previewPlayerPage.refreshKdp3</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="2" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>229</v>
+        <v>6</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="D103" s="2" t="str">
-        <f>CONCATENATE($D$97,C103)</f>
-        <v>wizard.previewPlayerPage.autoPreview</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="7" t="s">
-        <v>88</v>
+        <f>CONCATENATE($C$91,C103)</f>
+        <v>wizard.featurePage.</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D104" s="2" t="str">
+        <f>CONCATENATE($D$103,C104)</f>
+        <v>wizard.featurePage.accordi</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="2" t="str">
+        <f>CONCATENATE($D$103,C105)</f>
+        <v>wizard.featurePage.featureScreen</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D106" s="2" t="str">
+        <f>CONCATENATE($D$103,C106)</f>
+        <v>wizard.featurePage.keyValueBox</v>
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="5" t="s">
-        <v>89</v>
+      <c r="A108" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D109" s="2" t="str">
-        <f>CONCATENATE($C$108,C109)</f>
-        <v>content.manage.entryTable</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D111" s="2" t="str">
-        <f>CONCATENATE($C$108,C111)</f>
-        <v>content.manage.toolBar.</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="D108" s="2" t="str">
+        <f>CONCATENATE($C$91,C108)</f>
+        <v>wizard.advertizingPage</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D110" s="2" t="str">
+        <f>CONCATENATE($C$91,C110)</f>
+        <v>wizard.stylePage</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="2" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>97</v>
+        <v>249</v>
       </c>
       <c r="D112" s="2" t="str">
-        <f>CONCATENATE($D$111,C112)</f>
-        <v>content.manage.toolBar.deleteBtn</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+        <f>CONCATENATE($C$91,C112)</f>
+        <v>wizard.contentPage.</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>96</v>
+        <v>253</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="D113" s="2" t="str">
-        <f t="shared" ref="D113:D117" si="6">CONCATENATE($D$111,C113)</f>
-        <v>content.manage.toolBar.newStreamBtn</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D114" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>content.manage.toolBar.download</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <f>CONCATENATE($D$112,C113)</f>
+        <v>wizard.contentPage.all</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>103</v>
+        <v>240</v>
       </c>
       <c r="D115" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>content.manage.toolBar.tagsCombo</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+        <f>CONCATENATE($C$91,C115)</f>
+        <v>wizard.previewPlayerPage.</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>107</v>
+        <v>250</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>106</v>
+        <v>251</v>
       </c>
       <c r="D116" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>content.manage.toolBar.playlistCombo</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+        <f t="shared" ref="D116:D121" si="7">CONCATENATE($D$115,C116)</f>
+        <v>wizard.previewPlayerPage.controls</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
-        <v>109</v>
+        <v>239</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>104</v>
+        <v>211</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="D117" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>content.manage.toolBar.moreOption</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <f t="shared" si="7"/>
+        <v>wizard.previewPlayerPage.openClosePreview</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D118" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>wizard.previewPlayerPage.kdpWidth</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="2" t="s">
-        <v>111</v>
+        <v>246</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>85</v>
+        <v>233</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>114</v>
+        <v>242</v>
       </c>
       <c r="D119" s="2" t="str">
-        <f>CONCATENATE($C$108,C119)</f>
-        <v>content.manage.filter.</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <f t="shared" si="7"/>
+        <v>wizard.previewPlayerPage.kdpHeight</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="2" t="s">
-        <v>115</v>
+        <v>247</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>6</v>
+        <v>211</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>113</v>
+        <v>243</v>
       </c>
       <c r="D120" s="2" t="str">
-        <f>CONCATENATE($D$119,C120)</f>
-        <v>content.manage.filter.searchBox</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+        <f t="shared" si="7"/>
+        <v>wizard.previewPlayerPage.refreshKdp3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="2" t="s">
-        <v>117</v>
+        <v>248</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>6</v>
+        <v>229</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="D121" s="2" t="str">
-        <f t="shared" ref="D121:D129" si="7">CONCATENATE($D$119,C121)</f>
-        <v>content.manage.filter.dateCont</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D122" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>content.manage.filter.mediaTypes</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D123" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.conversionStatus</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D124" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.durationStatus</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D125" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.scheduling</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>6</v>
+        <v>wizard.previewPlayerPage.autoPreview</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D126" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.moderationStatus</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="2" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="D127" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.accessControl</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D128" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.transcodingFlavor</v>
+        <f>CONCATENATE($C$126,C127)</f>
+        <v>content.manage.entryTable</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="2" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="D129" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>content.manage.filter.categoriesBox</v>
+        <f>CONCATENATE($C$126,C129)</f>
+        <v>content.manage.toolBar.</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D130" s="2" t="str">
+        <f>CONCATENATE($D$129,C130)</f>
+        <v>content.manage.toolBar.deleteBtn</v>
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="5" t="s">
-        <v>135</v>
+      <c r="A131" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="D131" s="2" t="str">
+        <f t="shared" ref="D131:D135" si="8">CONCATENATE($D$129,C131)</f>
+        <v>content.manage.toolBar.newStreamBtn</v>
       </c>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D132" s="2" t="str">
-        <f>CONCATENATE($C$131,C132)</f>
-        <v>content.moderation.filter.</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>99</v>
+        <f t="shared" si="8"/>
+        <v>content.manage.toolBar.download</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D133" s="2" t="str">
-        <f>CONCATENATE($D$119,C133)</f>
-        <v>content.manage.filter.searchBox</v>
+        <f t="shared" si="8"/>
+        <v>content.manage.toolBar.tagsCombo</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D134" s="2" t="str">
-        <f t="shared" ref="D134:D142" si="8">CONCATENATE($D$119,C134)</f>
-        <v>content.manage.filter.dateCont</v>
+        <f t="shared" si="8"/>
+        <v>content.manage.toolBar.playlistCombo</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D135" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>content.manage.filter.mediaTypes</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D136" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.conversionStatus</v>
+        <v>content.manage.toolBar.moreOption</v>
       </c>
     </row>
     <row r="137" spans="1:6">
       <c r="A137" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D137" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.durationStatus</v>
+        <f>CONCATENATE($C$126,C137)</f>
+        <v>content.manage.filter.</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="A138" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D138" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.scheduling</v>
+        <f>CONCATENATE($D$137,C138)</f>
+        <v>content.manage.filter.searchBox</v>
       </c>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D139" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.moderationStatus</v>
+        <f t="shared" ref="D139:D147" si="9">CONCATENATE($D$137,C139)</f>
+        <v>content.manage.filter.dateCont</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D140" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.accessControl</v>
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.mediaTypes</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D141" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.transcodingFlavor</v>
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.conversionStatus</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D142" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.filter.categoriesBox</v>
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D143" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.scheduling</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="2" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="D144" s="2" t="str">
-        <f>CONCATENATE($C$131,C144)</f>
-        <v>content.moderation.entryTable</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.moderationStatus</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="2" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="D145" s="2" t="str">
-        <f>CONCATENATE($C$131,C145)</f>
-        <v>content.moderation.toolBar.</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.accessControl</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f>CONCATENATE($D$145,C146)</f>
-        <v>content.moderation.toolBar.approveSelected</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f>CONCATENATE($D$145,C147)</f>
-        <v>content.moderation.toolBar.rejectSelected</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
+        <f t="shared" si="9"/>
+        <v>content.manage.filter.categoriesBox</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="2" t="s">
         <v>111</v>
       </c>
@@ -2851,14 +2995,20 @@
         <v>85</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D150" s="2" t="str">
         <f>CONCATENATE($C$149,C150)</f>
-        <v>content.playlists.filter</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
+        <v>content.moderation.filter.</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" s="2" t="s">
         <v>115</v>
       </c>
@@ -2866,14 +3016,14 @@
         <v>6</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="D151" s="2" t="str">
-        <f>CONCATENATE($D$150,C151)</f>
-        <v>content.playlists.filterfreeText</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
+        <f>CONCATENATE($D$137,C151)</f>
+        <v>content.manage.filter.searchBox</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" s="2" t="s">
         <v>117</v>
       </c>
@@ -2884,475 +3034,708 @@
         <v>116</v>
       </c>
       <c r="D152" s="2" t="str">
-        <f>CONCATENATE($D$150,C152)</f>
-        <v>content.playlists.filterdateCont</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
+        <f t="shared" ref="D152:D160" si="10">CONCATENATE($D$137,C152)</f>
+        <v>content.manage.filter.dateCont</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D153" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.mediaTypes</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D154" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.conversionStatus</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D155" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D156" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.scheduling</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D157" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.moderationStatus</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D158" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.accessControl</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D159" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D160" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>content.manage.filter.categoriesBox</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D154" s="2" t="str">
-        <f t="shared" ref="D154:D160" si="9">CONCATENATE($C$149,C154)</f>
-        <v>content.playlists.entryTableContainer</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="A155" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C155" s="2" t="s">
+      <c r="B162" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D162" s="2" t="str">
+        <f>CONCATENATE($C$149,C162)</f>
+        <v>content.moderation.entryTable</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D155" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.playlists.toolBar.</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="A156" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D156" s="2" t="str">
-        <f>CONCATENATE($D$155,C156)</f>
-        <v>content.playlists.toolBar.deleteBtn</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D158" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.playlists.actionsBox</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D159" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.playlists.addManualPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D160" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.playlists.addRuleBasedPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="D163" s="2" t="str">
-        <f>CONCATENATE($C$162,C163)</f>
-        <v>content.syndication.feedsTable</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
+        <f>CONCATENATE($C$149,C163)</f>
+        <v>content.moderation.toolBar.</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="2" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>CONCATENATE($C$162,C164)</f>
-        <v>content.syndication.deleteExSynBtn</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
+        <f>CONCATENATE($D$163,C164)</f>
+        <v>content.moderation.toolBar.approveSelected</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f t="shared" ref="D165:D166" si="10">CONCATENATE($C$162,C165)</f>
-        <v>content.syndication.actionsBox</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
-      <c r="A166" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D166" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.syndication.addBtn</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="8" t="s">
-        <v>172</v>
+        <f>CONCATENATE($D$163,C165)</f>
+        <v>content.moderation.toolBar.rejectSelected</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="A170" s="5" t="s">
-        <v>158</v>
+        <v>111</v>
+      </c>
+      <c r="D168" s="2" t="str">
+        <f>CONCATENATE($C$167,C168)</f>
+        <v>content.playlists.filter</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D169" s="2" t="str">
+        <f>CONCATENATE($D$168,C169)</f>
+        <v>content.playlists.filterfreeText</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="A171" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D171" s="2" t="str">
-        <f>CONCATENATE($C$170,C171)</f>
-        <v>content.upload.kcwBox</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
+        <v>116</v>
+      </c>
+      <c r="D170" s="2" t="str">
+        <f>CONCATENATE($D$168,C170)</f>
+        <v>content.playlists.filterdateCont</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" s="2" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f t="shared" ref="D172:D173" si="11">CONCATENATE($C$170,C172)</f>
-        <v>content.upload.profilesCb</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6">
+        <f t="shared" ref="D172:D178" si="11">CONCATENATE($C$167,C172)</f>
+        <v>content.playlists.entryTableContainer</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" s="2" t="s">
-        <v>169</v>
+        <v>93</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="D173" s="2" t="str">
         <f t="shared" si="11"/>
+        <v>content.playlists.toolBar.</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D174" s="2" t="str">
+        <f>CONCATENATE($D$173,C174)</f>
+        <v>content.playlists.toolBar.deleteBtn</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D176" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>content.playlists.actionsBox</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D177" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>content.playlists.addManualPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D178" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>content.playlists.addRuleBasedPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D181" s="2" t="str">
+        <f>CONCATENATE($C$180,C181)</f>
+        <v>content.syndication.feedsTable</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D182" s="2" t="str">
+        <f>CONCATENATE($C$180,C182)</f>
+        <v>content.syndication.deleteExSynBtn</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D183" s="2" t="str">
+        <f t="shared" ref="D183:D184" si="12">CONCATENATE($C$180,C183)</f>
+        <v>content.syndication.actionsBox</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D184" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>content.syndication.addBtn</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D189" s="2" t="str">
+        <f>CONCATENATE($C$188,C189)</f>
+        <v>content.upload.kcwBox</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D190" s="2" t="str">
+        <f t="shared" ref="D190:D191" si="13">CONCATENATE($C$188,C190)</f>
+        <v>content.upload.profilesCb</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D191" s="2" t="str">
+        <f t="shared" si="13"/>
         <v>content.upload.kcwBtn</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
-      <c r="A174" s="2" t="s">
+    <row r="192" spans="1:6">
+      <c r="A192" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C192" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D174" s="2" t="str">
-        <f t="shared" ref="D174:D175" si="12">CONCATENATE($C$170,C174)</f>
+      <c r="D192" s="2" t="str">
+        <f t="shared" ref="D192:D193" si="14">CONCATENATE($C$188,C192)</f>
         <v>content.upload.bulkUploadBox</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
-      <c r="A175" s="2" t="s">
+    <row r="193" spans="1:7">
+      <c r="A193" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B193" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C193" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D175" s="2" t="str">
-        <f t="shared" si="12"/>
+      <c r="D193" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>content.upload.submitBtn</v>
       </c>
     </row>
-    <row r="177" spans="1:7">
-      <c r="A177" s="8" t="s">
+    <row r="195" spans="1:7">
+      <c r="A195" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C195" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E177" s="2" t="s">
+      <c r="E195" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F177" s="2" t="s">
+      <c r="F195" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G177" s="2" t="s">
+      <c r="G195" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="178" spans="1:7">
-      <c r="A178" s="2" t="s">
+    <row r="196" spans="1:7">
+      <c r="A196" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C178" s="2" t="s">
+      <c r="B196" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D178" s="2" t="str">
-        <f>CONCATENATE($C$177,C178)</f>
+      <c r="D196" s="2" t="str">
+        <f>CONCATENATE($C$195,C196)</f>
         <v>entryDrilldown.entryMetaData.</v>
       </c>
     </row>
-    <row r="179" spans="1:7">
-      <c r="A179" s="2" t="s">
+    <row r="197" spans="1:7">
+      <c r="A197" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B197" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="C197" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D179" s="2" t="str">
-        <f>CONCATENATE($D$178,C179)</f>
+      <c r="D197" s="2" t="str">
+        <f>CONCATENATE($D$196,C197)</f>
         <v>entryDrilldown.entryMetaData.name_input</v>
       </c>
     </row>
-    <row r="180" spans="1:7">
-      <c r="A180" s="2" t="s">
+    <row r="198" spans="1:7">
+      <c r="A198" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B198" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C198" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D180" s="2" t="str">
-        <f t="shared" ref="D180:D183" si="13">CONCATENATE($D$178,C180)</f>
+      <c r="D198" s="2" t="str">
+        <f t="shared" ref="D198:D201" si="15">CONCATENATE($D$196,C198)</f>
         <v>entryDrilldown.entryMetaData.descriptionTi</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
-      <c r="A181" s="2" t="s">
+    <row r="199" spans="1:7">
+      <c r="A199" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B199" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C199" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D181" s="2" t="str">
-        <f t="shared" si="13"/>
+      <c r="D199" s="2" t="str">
+        <f t="shared" si="15"/>
         <v>entryDrilldown.entryMetaData.tagsTi</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
-      <c r="A182" s="2" t="s">
+    <row r="200" spans="1:7">
+      <c r="A200" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D182" s="2" t="str">
-        <f t="shared" si="13"/>
+      <c r="D200" s="2" t="str">
+        <f t="shared" si="15"/>
         <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
       </c>
     </row>
-    <row r="183" spans="1:7">
-      <c r="A183" s="2" t="s">
+    <row r="201" spans="1:7">
+      <c r="A201" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C183" s="2" t="s">
+      <c r="B201" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D183" s="2" t="str">
-        <f t="shared" si="13"/>
+      <c r="D201" s="2" t="str">
+        <f t="shared" si="15"/>
         <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
       </c>
     </row>
-    <row r="185" spans="1:7">
-      <c r="A185" s="2" t="s">
+    <row r="203" spans="1:7">
+      <c r="A203" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C185" s="2" t="s">
+      <c r="B203" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D185" s="2" t="str">
-        <f>CONCATENATE($C$177,C185)</f>
+      <c r="D203" s="2" t="str">
+        <f>CONCATENATE($C$195,C203)</f>
         <v>entryDrilldown.entryAcp.</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
-      <c r="A186" s="2" t="s">
+    <row r="204" spans="1:7">
+      <c r="A204" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B204" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C204" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D186" s="2" t="str">
-        <f>CONCATENATE($D$185,C186)</f>
+      <c r="D204" s="2" t="str">
+        <f>CONCATENATE($D$203,C204)</f>
         <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
-      <c r="A187" s="2" t="s">
+    <row r="205" spans="1:7">
+      <c r="A205" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B205" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C205" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D187" s="2" t="str">
-        <f>CONCATENATE($D$185,C187)</f>
+      <c r="D205" s="2" t="str">
+        <f>CONCATENATE($D$203,C205)</f>
         <v>entryDrilldown.entryAcp.addBtn</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
-      <c r="A189" s="2" t="s">
+    <row r="207" spans="1:7">
+      <c r="A207" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C189" s="2" t="s">
+      <c r="B207" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D189" s="2" t="str">
-        <f>CONCATENATE($C$177,C189)</f>
+      <c r="D207" s="2" t="str">
+        <f>CONCATENATE($C$195,C207)</f>
         <v>entryDrilldown.customData</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
-      <c r="A191" s="2" t="s">
+    <row r="209" spans="1:7">
+      <c r="A209" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C191" s="2" t="s">
+      <c r="B209" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D191" s="2" t="str">
-        <f>CONCATENATE($C$177,C191)</f>
+      <c r="D209" s="2" t="str">
+        <f>CONCATENATE($C$195,C209)</f>
         <v>entryDrilldown.entryAsstes</v>
       </c>
-      <c r="E191" s="2" t="s">
+      <c r="E209" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F191" s="2" t="s">
+      <c r="F209" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G191" s="2" t="s">
+      <c r="G209" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
-      <c r="A193" s="8" t="s">
+    <row r="211" spans="1:7">
+      <c r="A211" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C211" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E193" s="2" t="s">
+      <c r="E211" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F193" s="2" t="s">
+      <c r="F211" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
-      <c r="A194" s="8" t="s">
+    <row r="212" spans="1:7">
+      <c r="A212" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C212" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E194" s="2" t="s">
+      <c r="E212" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F194" s="2" t="s">
+      <c r="F212" s="2" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
account / metadata / drilldown mapping
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@53809 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="325">
   <si>
     <t>Dashboard</t>
   </si>
@@ -949,6 +949,48 @@
   </si>
   <si>
     <t>enableNotificationsTable</t>
+  </si>
+  <si>
+    <t>add / edit metadata field popup</t>
+  </si>
+  <si>
+    <t>fullDescriptionInput</t>
+  </si>
+  <si>
+    <t>descriptionInput</t>
+  </si>
+  <si>
+    <t>appearInSearchList</t>
+  </si>
+  <si>
+    <t>maxValuesList</t>
+  </si>
+  <si>
+    <t>optionalValuesInput</t>
+  </si>
+  <si>
+    <t>fieldTypeList</t>
+  </si>
+  <si>
+    <t>fieldNameInput</t>
+  </si>
+  <si>
+    <t>field name</t>
+  </si>
+  <si>
+    <t>field type</t>
+  </si>
+  <si>
+    <t>optional values if needed</t>
+  </si>
+  <si>
+    <t>field description</t>
+  </si>
+  <si>
+    <t>field full description</t>
+  </si>
+  <si>
+    <t>customDataDrilldown.</t>
   </si>
 </sst>
 </file>
@@ -1334,11 +1376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G216"/>
+  <dimension ref="A1:G226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79:D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1734,7 +1776,7 @@
         <v>269</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f>CONCATENATE($C$37,C38)</f>
+        <f t="shared" ref="D38:D59" si="3">CONCATENATE($C$37,C38)</f>
         <v>acDrilldown.profileNameTi</v>
       </c>
     </row>
@@ -1749,7 +1791,7 @@
         <v>271</v>
       </c>
       <c r="D39" s="2" t="str">
-        <f>CONCATENATE($C$37,C39)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.descriptionTa</v>
       </c>
     </row>
@@ -1761,7 +1803,7 @@
         <v>273</v>
       </c>
       <c r="D40" s="2" t="str">
-        <f>CONCATENATE($C$37,C40)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.anySiteRaddioBtn</v>
       </c>
     </row>
@@ -1773,7 +1815,7 @@
         <v>274</v>
       </c>
       <c r="D41" s="2" t="str">
-        <f>CONCATENATE($C$37,C41)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.approvedSitesRadioBtn</v>
       </c>
     </row>
@@ -1788,7 +1830,7 @@
         <v>275</v>
       </c>
       <c r="D42" s="2" t="str">
-        <f>CONCATENATE($C$37,C42)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.approvedDomainsList</v>
       </c>
     </row>
@@ -1803,7 +1845,7 @@
         <v>284</v>
       </c>
       <c r="D43" s="2" t="str">
-        <f>CONCATENATE($C$37,C43)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.addAuthorisedBtn</v>
       </c>
     </row>
@@ -1818,7 +1860,7 @@
         <v>283</v>
       </c>
       <c r="D44" s="2" t="str">
-        <f>CONCATENATE($C$37,C44)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.removeAuthorisedBtn</v>
       </c>
     </row>
@@ -1830,7 +1872,7 @@
         <v>280</v>
       </c>
       <c r="D45" s="2" t="str">
-        <f>CONCATENATE($C$37,C45)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedSitesRadioBtn</v>
       </c>
     </row>
@@ -1845,7 +1887,7 @@
         <v>281</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f>CONCATENATE($C$37,C46)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedDomainsList</v>
       </c>
     </row>
@@ -1860,7 +1902,7 @@
         <v>285</v>
       </c>
       <c r="D47" s="2" t="str">
-        <f>CONCATENATE($C$37,C47)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.addUnauthorisedBtn</v>
       </c>
     </row>
@@ -1875,7 +1917,7 @@
         <v>286</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f>CONCATENATE($C$37,C48)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.removeUnauthorisedBtn</v>
       </c>
     </row>
@@ -1887,7 +1929,7 @@
         <v>287</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f>CONCATENATE($C$37,C49)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.allCountriesRaddioBtn</v>
       </c>
     </row>
@@ -1899,7 +1941,7 @@
         <v>288</v>
       </c>
       <c r="D50" s="2" t="str">
-        <f>CONCATENATE($C$37,C50)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.approvedCountiesRadioBtn</v>
       </c>
     </row>
@@ -1911,7 +1953,7 @@
         <v>289</v>
       </c>
       <c r="D51" s="2" t="str">
-        <f>CONCATENATE($C$37,C51)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.approvedCountriesList</v>
       </c>
     </row>
@@ -1923,7 +1965,7 @@
         <v>290</v>
       </c>
       <c r="D52" s="2" t="str">
-        <f>CONCATENATE($C$37,C52)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.addRemoveCountriesBtn</v>
       </c>
     </row>
@@ -1935,7 +1977,7 @@
         <v>291</v>
       </c>
       <c r="D53" s="2" t="str">
-        <f>CONCATENATE($C$37,C53)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedCountriesRadioBtn</v>
       </c>
     </row>
@@ -1947,7 +1989,7 @@
         <v>292</v>
       </c>
       <c r="D54" s="2" t="str">
-        <f>CONCATENATE($C$37,C54)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedCountriesList</v>
       </c>
     </row>
@@ -1959,7 +2001,7 @@
         <v>293</v>
       </c>
       <c r="D55" s="2" t="str">
-        <f>CONCATENATE($C$37,C55)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.restrictCountriesLinkButton</v>
       </c>
     </row>
@@ -1974,7 +2016,7 @@
         <v>294</v>
       </c>
       <c r="D56" s="2" t="str">
-        <f>CONCATENATE($C$37,C56)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.secureKSCBBtn</v>
       </c>
     </row>
@@ -1989,7 +2031,7 @@
         <v>296</v>
       </c>
       <c r="D57" s="2" t="str">
-        <f>CONCATENATE($C$37,C57)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.freePerviewCBBtn</v>
       </c>
     </row>
@@ -2004,7 +2046,7 @@
         <v>298</v>
       </c>
       <c r="D58" s="2" t="str">
-        <f>CONCATENATE($C$37,C58)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.freePreviewDuration</v>
       </c>
     </row>
@@ -2019,7 +2061,7 @@
         <v>171</v>
       </c>
       <c r="D59" s="2" t="str">
-        <f>CONCATENATE($C$37,C59)</f>
+        <f t="shared" si="3"/>
         <v>acDrilldown.submitBtn</v>
       </c>
     </row>
@@ -2057,7 +2099,7 @@
         <v>48</v>
       </c>
       <c r="D63" s="2" t="str">
-        <f t="shared" ref="D63:D64" si="3">CONCATENATE($C$61,C63)</f>
+        <f t="shared" ref="D63:D64" si="4">CONCATENATE($C$61,C63)</f>
         <v>account.transcodingswitchModeBtn</v>
       </c>
     </row>
@@ -2072,11 +2114,11 @@
         <v>49</v>
       </c>
       <c r="D64" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>account.transcodingsaveButton</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:6">
       <c r="A67" s="5" t="s">
         <v>51</v>
       </c>
@@ -2084,7 +2126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
         <v>53</v>
       </c>
@@ -2099,7 +2141,7 @@
         <v>account.upgrade.customFieldsTable</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
         <v>58</v>
       </c>
@@ -2114,7 +2156,7 @@
         <v>account.upgrade.addFieldButton</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
         <v>57</v>
       </c>
@@ -2129,7 +2171,7 @@
         <v>account.upgrade.deleteCustomDataField</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:6">
       <c r="A72" s="5" t="s">
         <v>304</v>
       </c>
@@ -2137,7 +2179,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:6">
       <c r="A73" s="4" t="s">
         <v>305</v>
       </c>
@@ -2152,7 +2194,7 @@
         <v>account.metadata.deleteCustomDataField</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
         <v>307</v>
       </c>
@@ -2163,11 +2205,11 @@
         <v>303</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f t="shared" ref="D74:D76" si="4">CONCATENATE($C$72,C74)</f>
+        <f t="shared" ref="D74:D86" si="5">CONCATENATE($C$72,C74)</f>
         <v>account.metadata.actionBox</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>308</v>
       </c>
@@ -2178,11 +2220,11 @@
         <v>55</v>
       </c>
       <c r="D75" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>account.metadata.addFieldButton</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
         <v>309</v>
       </c>
@@ -2193,1665 +2235,1807 @@
         <v>52</v>
       </c>
       <c r="D76" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>account.metadata.customFieldsTable</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="5" t="s">
-        <v>63</v>
+    <row r="77" spans="1:6">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="2" t="s">
-        <v>32</v>
+        <v>262</v>
+      </c>
+      <c r="D79" s="2" t="str">
+        <f>CONCATENATE($C$78,C79)</f>
+        <v>customDataDrilldown.saveBtn</v>
+      </c>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="4" t="s">
+        <v>323</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>32</v>
+        <v>312</v>
       </c>
       <c r="D80" s="2" t="str">
-        <f>CONCATENATE($C$79,C80)</f>
-        <v>admin.users.table</v>
-      </c>
+        <f t="shared" ref="D80:D86" si="6">CONCATENATE($C$78,C80)</f>
+        <v>customDataDrilldown.fullDescriptionInput</v>
+      </c>
+      <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:7">
-      <c r="A81" s="2" t="s">
-        <v>66</v>
+      <c r="A81" s="4" t="s">
+        <v>322</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>65</v>
+        <v>313</v>
       </c>
       <c r="D81" s="2" t="str">
-        <f>CONCATENATE($C$79,C81)</f>
-        <v>admin.users.addBtn</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.descriptionInput</v>
+      </c>
+      <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:7">
-      <c r="A82" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="A82" s="4"/>
       <c r="B82" s="2" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>67</v>
+        <v>314</v>
       </c>
       <c r="D82" s="2" t="str">
-        <f>CONCATENATE($C$79,C82)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.appearInSearchList</v>
+      </c>
+      <c r="F82" s="4"/>
     </row>
     <row r="83" spans="1:7">
-      <c r="A83" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>82</v>
+      <c r="A83" s="4"/>
+      <c r="B83" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>32</v>
+        <v>315</v>
       </c>
       <c r="D83" s="2" t="str">
-        <f>CONCATENATE($C$79,C83)</f>
-        <v>admin.users.table</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="5" t="s">
-        <v>64</v>
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.maxValuesList</v>
+      </c>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D84" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.optionalValuesInput</v>
+      </c>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:7" ht="12" customHeight="1">
+      <c r="A85" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="D85" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.fieldTypeList</v>
+      </c>
+      <c r="F85" s="4"/>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>customDataDrilldown.fieldNameInput</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="2" t="str">
-        <f>CONCATENATE($C$79,C86)</f>
+      <c r="D90" s="2" t="str">
+        <f>CONCATENATE($C$89,C90)</f>
         <v>admin.users.table</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="2" t="s">
+    <row r="91" spans="1:7">
+      <c r="A91" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D87" s="2" t="str">
-        <f>CONCATENATE($C$79,C87)</f>
+      <c r="D91" s="2" t="str">
+        <f>CONCATENATE($C$89,C91)</f>
         <v>admin.users.addBtn</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="2" t="s">
+    <row r="92" spans="1:7">
+      <c r="A92" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D88" s="2" t="str">
-        <f>CONCATENATE($C$79,C88)</f>
+      <c r="D92" s="2" t="str">
+        <f>CONCATENATE($C$89,C92)</f>
         <v>admin.users.actionButtonsContainer</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="4" t="s">
+    <row r="93" spans="1:7">
+      <c r="A93" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="2" t="str">
-        <f>CONCATENATE($C$79,C89)</f>
+      <c r="D93" s="2" t="str">
+        <f>CONCATENATE($C$89,C93)</f>
         <v>admin.users.table</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F89" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G89" s="2" t="s">
+      <c r="F93" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G93" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D94" s="2" t="str">
-        <f>CONCATENATE($C$93,C94)</f>
-        <v>studio.playerList.templatesHolder</v>
-      </c>
-    </row>
     <row r="95" spans="1:7">
-      <c r="A95" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>85</v>
+      <c r="A95" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" s="2" t="str">
+        <f>CONCATENATE($C$89,C96)</f>
+        <v>admin.users.table</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D97" s="2" t="str">
+        <f>CONCATENATE($C$89,C97)</f>
+        <v>admin.users.addBtn</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="2" t="str">
+        <f>CONCATENATE($C$89,C98)</f>
+        <v>admin.users.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="2" t="str">
+        <f>CONCATENATE($C$89,C99)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" s="2" t="str">
+        <f>CONCATENATE($C$103,C104)</f>
+        <v>studio.playerList.templatesHolder</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D96" s="2" t="str">
-        <f>CONCATENATE($C$95,C96)</f>
+      <c r="D106" s="2" t="str">
+        <f>CONCATENATE($C$105,C106)</f>
         <v>wizard.wizardSaveBtn</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="1" t="s">
+    <row r="107" spans="1:7">
+      <c r="A107" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97" s="1" t="s">
+      <c r="B107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D97" s="1" t="str">
-        <f t="shared" ref="D97" si="5">CONCATENATE($C$95,C97)</f>
+      <c r="D107" s="1" t="str">
+        <f t="shared" ref="D107" si="7">CONCATENATE($C$105,C107)</f>
         <v>wizard.templatePage.</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="1" t="s">
+    <row r="108" spans="1:7">
+      <c r="A108" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="1" t="s">
+      <c r="B108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D98" s="1" t="str">
-        <f t="shared" ref="D98:D105" si="6">CONCATENATE($D$97,C98)</f>
+      <c r="D108" s="1" t="str">
+        <f t="shared" ref="D108:D115" si="8">CONCATENATE($D$107,C108)</f>
         <v>wizard.templatePage.all</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="1" t="s">
+    <row r="109" spans="1:7">
+      <c r="A109" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D99" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D109" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.playerName</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="1" t="s">
+    <row r="110" spans="1:7">
+      <c r="A110" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D100" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D110" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.keepOriginalRatio</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="1" t="s">
+    <row r="111" spans="1:7">
+      <c r="A111" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D101" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D111" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.streachMediaToFitPlayer</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="1" t="s">
+    <row r="112" spans="1:7">
+      <c r="A112" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D102" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D112" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.templateAutoPlay</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="1" t="s">
+    <row r="113" spans="1:6">
+      <c r="A113" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D103" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D113" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.templateAutoMute</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="1" t="s">
+    <row r="114" spans="1:6">
+      <c r="A114" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D104" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D114" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.playlistAutoContinue</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
-      <c r="A105" s="1" t="s">
+    <row r="115" spans="1:6">
+      <c r="A115" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D105" s="1" t="str">
-        <f t="shared" si="6"/>
+      <c r="D115" s="1" t="str">
+        <f t="shared" si="8"/>
         <v>wizard.templatePage.playlistImagesInterval</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="2" t="s">
+    <row r="117" spans="1:6">
+      <c r="A117" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C107" s="2" t="s">
+      <c r="B117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D107" s="2" t="str">
-        <f>CONCATENATE($C$95,C107)</f>
+      <c r="D117" s="2" t="str">
+        <f>CONCATENATE($C$105,C117)</f>
         <v>wizard.featurePage.</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="E117" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="3" t="s">
+    <row r="118" spans="1:6">
+      <c r="A118" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D108" s="2" t="str">
-        <f>CONCATENATE($D$107,C108)</f>
+      <c r="D118" s="2" t="str">
+        <f>CONCATENATE($D$117,C118)</f>
         <v>wizard.featurePage.accordi</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="3" t="s">
+    <row r="119" spans="1:6">
+      <c r="A119" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="2" t="s">
+      <c r="B119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D109" s="2" t="str">
-        <f>CONCATENATE($D$107,C109)</f>
+      <c r="D119" s="2" t="str">
+        <f>CONCATENATE($D$117,C119)</f>
         <v>wizard.featurePage.featureScreen</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="3" t="s">
+    <row r="120" spans="1:6">
+      <c r="A120" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110" s="2" t="s">
+      <c r="B120" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D110" s="2" t="str">
-        <f>CONCATENATE($D$107,C110)</f>
+      <c r="D120" s="2" t="str">
+        <f>CONCATENATE($D$117,C120)</f>
         <v>wizard.featurePage.keyValueBox</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
-      <c r="A112" s="2" t="s">
+    <row r="122" spans="1:6">
+      <c r="A122" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C112" s="2" t="s">
+      <c r="B122" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D112" s="2" t="str">
-        <f>CONCATENATE($C$95,C112)</f>
+      <c r="D122" s="2" t="str">
+        <f>CONCATENATE($C$105,C122)</f>
         <v>wizard.advertizingPage</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="2" t="s">
+    <row r="124" spans="1:6">
+      <c r="A124" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C114" s="2" t="s">
+      <c r="B124" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D114" s="2" t="str">
-        <f>CONCATENATE($C$95,C114)</f>
+      <c r="D124" s="2" t="str">
+        <f>CONCATENATE($C$105,C124)</f>
         <v>wizard.stylePage</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="2" t="s">
+    <row r="126" spans="1:6">
+      <c r="A126" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" s="2" t="s">
+      <c r="B126" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D116" s="2" t="str">
-        <f>CONCATENATE($C$95,C116)</f>
+      <c r="D126" s="2" t="str">
+        <f>CONCATENATE($C$105,C126)</f>
         <v>wizard.contentPage.</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="2" t="s">
+    <row r="127" spans="1:6">
+      <c r="A127" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="2" t="s">
+      <c r="B127" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D117" s="2" t="str">
-        <f>CONCATENATE($D$116,C117)</f>
+      <c r="D127" s="2" t="str">
+        <f>CONCATENATE($D$126,C127)</f>
         <v>wizard.contentPage.all</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="2" t="s">
+    <row r="129" spans="1:6">
+      <c r="A129" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="2" t="s">
+      <c r="B129" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D119" s="2" t="str">
-        <f>CONCATENATE($C$95,C119)</f>
+      <c r="D129" s="2" t="str">
+        <f>CONCATENATE($C$105,C129)</f>
         <v>wizard.previewPlayerPage.</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="2" t="s">
+    <row r="130" spans="1:6">
+      <c r="A130" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C120" s="2" t="s">
+      <c r="B130" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D120" s="2" t="str">
-        <f t="shared" ref="D120:D125" si="7">CONCATENATE($D$119,C120)</f>
+      <c r="D130" s="2" t="str">
+        <f t="shared" ref="D130:D135" si="9">CONCATENATE($D$129,C130)</f>
         <v>wizard.previewPlayerPage.controls</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D121" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>wizard.previewPlayerPage.openClosePreview</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D122" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>wizard.previewPlayerPage.kdpWidth</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D123" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>wizard.previewPlayerPage.kdpHeight</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D124" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>wizard.previewPlayerPage.refreshKdp3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D125" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>wizard.previewPlayerPage.autoPreview</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="2" t="s">
-        <v>91</v>
+        <v>239</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>32</v>
+        <v>211</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="D131" s="2" t="str">
-        <f>CONCATENATE($C$130,C131)</f>
-        <v>content.manage.entryTable</v>
+        <f t="shared" si="9"/>
+        <v>wizard.previewPlayerPage.openClosePreview</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D132" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>wizard.previewPlayerPage.kdpWidth</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" s="2" t="s">
-        <v>94</v>
+        <v>246</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>94</v>
+        <v>233</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>100</v>
+        <v>242</v>
       </c>
       <c r="D133" s="2" t="str">
-        <f>CONCATENATE($C$130,C133)</f>
-        <v>content.manage.toolBar.</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>99</v>
+        <f t="shared" si="9"/>
+        <v>wizard.previewPlayerPage.kdpHeight</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="2" t="s">
-        <v>95</v>
+        <v>247</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>22</v>
+        <v>211</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>97</v>
+        <v>243</v>
       </c>
       <c r="D134" s="2" t="str">
-        <f>CONCATENATE($D$133,C134)</f>
-        <v>content.manage.toolBar.deleteBtn</v>
+        <f t="shared" si="9"/>
+        <v>wizard.previewPlayerPage.refreshKdp3</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="2" t="s">
-        <v>96</v>
+        <v>248</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>110</v>
+        <v>244</v>
       </c>
       <c r="D135" s="2" t="str">
-        <f t="shared" ref="D135:D139" si="8">CONCATENATE($D$133,C135)</f>
-        <v>content.manage.toolBar.newStreamBtn</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D136" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.toolBar.download</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D137" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.toolBar.tagsCombo</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D138" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.toolBar.playlistCombo</v>
+        <f t="shared" si="9"/>
+        <v>wizard.previewPlayerPage.autoPreview</v>
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D139" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>content.manage.toolBar.moreOption</v>
+      <c r="A139" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="2" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D141" s="2" t="str">
-        <f>CONCATENATE($C$130,C141)</f>
-        <v>content.manage.filter.</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D142" s="2" t="str">
-        <f>CONCATENATE($D$141,C142)</f>
-        <v>content.manage.filter.searchBox</v>
+        <f>CONCATENATE($C$140,C141)</f>
+        <v>content.manage.entryTable</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D143" s="2" t="str">
-        <f t="shared" ref="D143:D151" si="9">CONCATENATE($D$141,C143)</f>
-        <v>content.manage.filter.dateCont</v>
+        <f>CONCATENATE($C$140,C143)</f>
+        <v>content.manage.toolBar.</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="2" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="D144" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.mediaTypes</v>
+        <f>CONCATENATE($D$143,C144)</f>
+        <v>content.manage.toolBar.deleteBtn</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="2" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D145" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.conversionStatus</v>
+        <f t="shared" ref="D145:D149" si="10">CONCATENATE($D$143,C145)</f>
+        <v>content.manage.toolBar.newStreamBtn</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.durationStatus</v>
+        <f t="shared" si="10"/>
+        <v>content.manage.toolBar.download</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="2" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.scheduling</v>
+        <f t="shared" si="10"/>
+        <v>content.manage.toolBar.tagsCombo</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D148" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.moderationStatus</v>
+        <f t="shared" si="10"/>
+        <v>content.manage.toolBar.playlistCombo</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="2" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D149" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.accessControl</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D150" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.transcodingFlavor</v>
+        <f t="shared" si="10"/>
+        <v>content.manage.toolBar.moreOption</v>
       </c>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D151" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>content.manage.filter.categoriesBox</v>
+        <f>CONCATENATE($C$140,C151)</f>
+        <v>content.manage.filter.</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D152" s="2" t="str">
+        <f>CONCATENATE($D$151,C152)</f>
+        <v>content.manage.filter.searchBox</v>
       </c>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="5" t="s">
-        <v>135</v>
+      <c r="A153" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>136</v>
+        <v>116</v>
+      </c>
+      <c r="D153" s="2" t="str">
+        <f t="shared" ref="D153:D161" si="11">CONCATENATE($D$151,C153)</f>
+        <v>content.manage.filter.dateCont</v>
       </c>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D154" s="2" t="str">
-        <f>CONCATENATE($C$153,C154)</f>
-        <v>content.moderation.filter.</v>
-      </c>
-      <c r="E154" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F154" s="2" t="s">
-        <v>99</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.mediaTypes</v>
       </c>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D155" s="2" t="str">
-        <f>CONCATENATE($D$141,C155)</f>
-        <v>content.manage.filter.searchBox</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.conversionStatus</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f t="shared" ref="D156:D164" si="10">CONCATENATE($D$141,C156)</f>
-        <v>content.manage.filter.dateCont</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.durationStatus</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.filter.mediaTypes</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.scheduling</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.filter.conversionStatus</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.moderationStatus</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D159" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.filter.durationStatus</v>
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.accessControl</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D160" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D161" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>content.manage.filter.categoriesBox</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D164" s="2" t="str">
+        <f>CONCATENATE($C$163,C164)</f>
+        <v>content.moderation.filter.</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D165" s="2" t="str">
+        <f>CONCATENATE($D$151,C165)</f>
+        <v>content.manage.filter.searchBox</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D166" s="2" t="str">
+        <f t="shared" ref="D166:D174" si="12">CONCATENATE($D$151,C166)</f>
+        <v>content.manage.filter.dateCont</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D167" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>content.manage.filter.mediaTypes</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D168" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>content.manage.filter.conversionStatus</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D169" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C160" s="2" t="s">
+      <c r="B170" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D160" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="D170" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>content.manage.filter.scheduling</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
-      <c r="A161" s="2" t="s">
+    <row r="171" spans="1:6">
+      <c r="A171" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C161" s="2" t="s">
+      <c r="B171" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D161" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="D171" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>content.manage.filter.moderationStatus</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
-      <c r="A162" s="2" t="s">
+    <row r="172" spans="1:6">
+      <c r="A172" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C162" s="2" t="s">
+      <c r="B172" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D162" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="D172" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>content.manage.filter.accessControl</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
-      <c r="A163" s="2" t="s">
+    <row r="173" spans="1:6">
+      <c r="A173" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C163" s="2" t="s">
+      <c r="B173" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D163" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="D173" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>content.manage.filter.transcodingFlavor</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
-      <c r="A164" s="2" t="s">
+    <row r="174" spans="1:6">
+      <c r="A174" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C164" s="2" t="s">
+      <c r="B174" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D164" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="D174" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>content.manage.filter.categoriesBox</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D166" s="2" t="str">
-        <f>CONCATENATE($C$153,C166)</f>
-        <v>content.moderation.entryTable</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4">
-      <c r="A167" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D167" s="2" t="str">
-        <f>CONCATENATE($C$153,C167)</f>
-        <v>content.moderation.toolBar.</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4">
-      <c r="A168" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D168" s="2" t="str">
-        <f>CONCATENATE($D$167,C168)</f>
-        <v>content.moderation.toolBar.approveSelected</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4">
-      <c r="A169" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D169" s="2" t="str">
-        <f>CONCATENATE($D$167,C169)</f>
-        <v>content.moderation.toolBar.rejectSelected</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="A172" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D172" s="2" t="str">
-        <f>CONCATENATE($C$171,C172)</f>
-        <v>content.playlists.filter</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
-      <c r="A173" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D173" s="2" t="str">
-        <f>CONCATENATE($D$172,C173)</f>
-        <v>content.playlists.filterfreeText</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D174" s="2" t="str">
-        <f>CONCATENATE($D$172,C174)</f>
-        <v>content.playlists.filterdateCont</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:6">
       <c r="A176" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="D176" s="2" t="str">
-        <f t="shared" ref="D176:D182" si="11">CONCATENATE($C$171,C176)</f>
-        <v>content.playlists.entryTableContainer</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
+        <f>CONCATENATE($C$163,C176)</f>
+        <v>content.moderation.entryTable</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.playlists.toolBar.</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
+        <f>CONCATENATE($C$163,C177)</f>
+        <v>content.moderation.toolBar.</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="2" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="D178" s="2" t="str">
         <f>CONCATENATE($D$177,C178)</f>
-        <v>content.playlists.toolBar.deleteBtn</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="A180" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D180" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.playlists.actionsBox</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
-      <c r="A181" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B181" s="2" t="s">
+        <v>content.moderation.toolBar.approveSelected</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C179" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D179" s="2" t="str">
+        <f>CONCATENATE($D$177,C179)</f>
+        <v>content.moderation.toolBar.rejectSelected</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="C181" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D181" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.playlists.addManualPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="2" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="D182" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.playlists.addRuleBasedPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6">
-      <c r="A184" s="5" t="s">
-        <v>150</v>
+        <f>CONCATENATE($C$181,C182)</f>
+        <v>content.playlists.filter</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D183" s="2" t="str">
+        <f>CONCATENATE($D$182,C183)</f>
+        <v>content.playlists.filterfreeText</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6">
-      <c r="A185" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D185" s="2" t="str">
-        <f>CONCATENATE($C$184,C185)</f>
-        <v>content.syndication.feedsTable</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6">
+        <v>116</v>
+      </c>
+      <c r="D184" s="2" t="str">
+        <f>CONCATENATE($D$182,C184)</f>
+        <v>content.playlists.filterdateCont</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="2" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D186" s="2" t="str">
-        <f>CONCATENATE($C$184,C186)</f>
-        <v>content.syndication.deleteExSynBtn</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6">
+        <f t="shared" ref="D186:D192" si="13">CONCATENATE($C$181,C186)</f>
+        <v>content.playlists.entryTableContainer</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="2" t="s">
-        <v>156</v>
+        <v>93</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="D187" s="2" t="str">
-        <f t="shared" ref="D187:D188" si="12">CONCATENATE($C$184,C187)</f>
-        <v>content.syndication.actionsBox</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6">
+        <f t="shared" si="13"/>
+        <v>content.playlists.toolBar.</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="2" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C188" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D188" s="2" t="str">
+        <f>CONCATENATE($D$187,C188)</f>
+        <v>content.playlists.toolBar.deleteBtn</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D190" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>content.playlists.actionsBox</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D191" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>content.playlists.addManualPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D192" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>content.playlists.addRuleBasedPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D195" s="2" t="str">
+        <f>CONCATENATE($C$194,C195)</f>
+        <v>content.syndication.feedsTable</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D196" s="2" t="str">
+        <f>CONCATENATE($C$194,C196)</f>
+        <v>content.syndication.deleteExSynBtn</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D197" s="2" t="str">
+        <f t="shared" ref="D197:D198" si="14">CONCATENATE($C$194,C197)</f>
+        <v>content.syndication.actionsBox</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C198" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D188" s="2" t="str">
-        <f t="shared" si="12"/>
+      <c r="D198" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>content.syndication.addBtn</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
-      <c r="A190" s="8" t="s">
+    <row r="200" spans="1:6">
+      <c r="A200" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E190" s="2" t="s">
+      <c r="E200" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F190" s="2" t="s">
+      <c r="F200" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
-      <c r="A192" s="5" t="s">
+    <row r="202" spans="1:6">
+      <c r="A202" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C202" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="193" spans="1:7">
-      <c r="A193" s="2" t="s">
+    <row r="203" spans="1:6">
+      <c r="A203" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C203" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D193" s="2" t="str">
-        <f>CONCATENATE($C$192,C193)</f>
+      <c r="D203" s="2" t="str">
+        <f>CONCATENATE($C$202,C203)</f>
         <v>content.upload.kcwBox</v>
       </c>
     </row>
-    <row r="194" spans="1:7">
-      <c r="A194" s="2" t="s">
+    <row r="204" spans="1:6">
+      <c r="A204" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B204" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C204" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D194" s="2" t="str">
-        <f t="shared" ref="D194:D195" si="13">CONCATENATE($C$192,C194)</f>
+      <c r="D204" s="2" t="str">
+        <f t="shared" ref="D204:D205" si="15">CONCATENATE($C$202,C204)</f>
         <v>content.upload.profilesCb</v>
       </c>
     </row>
-    <row r="195" spans="1:7">
-      <c r="A195" s="2" t="s">
+    <row r="205" spans="1:6">
+      <c r="A205" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B205" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C205" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D195" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.upload.kcwBtn</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7">
-      <c r="A196" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D196" s="2" t="str">
-        <f t="shared" ref="D196:D197" si="14">CONCATENATE($C$192,C196)</f>
-        <v>content.upload.bulkUploadBox</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7">
-      <c r="A197" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D197" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.upload.submitBtn</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7">
-      <c r="A199" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F199" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G199" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7">
-      <c r="A200" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D200" s="2" t="str">
-        <f>CONCATENATE($C$199,C200)</f>
-        <v>entryDrilldown.entryMetaData.</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7">
-      <c r="A201" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D201" s="2" t="str">
-        <f>CONCATENATE($D$200,C201)</f>
-        <v>entryDrilldown.entryMetaData.name_input</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D202" s="2" t="str">
-        <f t="shared" ref="D202:D205" si="15">CONCATENATE($D$200,C202)</f>
-        <v>entryDrilldown.entryMetaData.descriptionTi</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D203" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>entryDrilldown.entryMetaData.tagsTi</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D204" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="D205" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7">
+        <v>content.upload.kcwBtn</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D206" s="2" t="str">
+        <f t="shared" ref="D206:D207" si="16">CONCATENATE($C$202,C206)</f>
+        <v>content.upload.bulkUploadBox</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207" s="2" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="D207" s="2" t="str">
-        <f>CONCATENATE($C$199,C207)</f>
-        <v>entryDrilldown.entryAcp.</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D208" s="2" t="str">
-        <f>CONCATENATE($D$207,C208)</f>
-        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+        <f t="shared" si="16"/>
+        <v>content.upload.submitBtn</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>197</v>
+      <c r="A209" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D209" s="2" t="str">
-        <f>CONCATENATE($D$207,C209)</f>
-        <v>entryDrilldown.entryAcp.addBtn</v>
+        <v>179</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D210" s="2" t="str">
+        <f>CONCATENATE($C$209,C210)</f>
+        <v>entryDrilldown.entryMetaData.</v>
       </c>
     </row>
     <row r="211" spans="1:7">
       <c r="A211" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>CONCATENATE($C$199,C211)</f>
-        <v>entryDrilldown.customData</v>
+        <f>CONCATENATE($D$210,C211)</f>
+        <v>entryDrilldown.entryMetaData.name_input</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D212" s="2" t="str">
+        <f t="shared" ref="D212:D215" si="17">CONCATENATE($D$210,C212)</f>
+        <v>entryDrilldown.entryMetaData.descriptionTi</v>
       </c>
     </row>
     <row r="213" spans="1:7">
       <c r="A213" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D213" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>entryDrilldown.entryMetaData.tagsTi</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D214" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D215" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D217" s="2" t="str">
+        <f>CONCATENATE($C$209,C217)</f>
+        <v>entryDrilldown.entryAcp.</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D218" s="2" t="str">
+        <f>CONCATENATE($D$217,C218)</f>
+        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D219" s="2" t="str">
+        <f>CONCATENATE($D$217,C219)</f>
+        <v>entryDrilldown.entryAcp.addBtn</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D221" s="2" t="str">
+        <f>CONCATENATE($C$209,C221)</f>
+        <v>entryDrilldown.customData</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C213" s="2" t="s">
+      <c r="B223" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D213" s="2" t="str">
-        <f>CONCATENATE($C$199,C213)</f>
+      <c r="D223" s="2" t="str">
+        <f>CONCATENATE($C$209,C223)</f>
         <v>entryDrilldown.entryAsstes</v>
       </c>
-      <c r="E213" s="2" t="s">
+      <c r="E223" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F213" s="2" t="s">
+      <c r="F223" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G213" s="2" t="s">
+      <c r="G223" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
-      <c r="A215" s="8" t="s">
+    <row r="225" spans="1:6">
+      <c r="A225" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="C225" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E215" s="2" t="s">
+      <c r="E225" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F215" s="2" t="s">
+      <c r="F225" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
-      <c r="A216" s="8" t="s">
+    <row r="226" spans="1:6">
+      <c r="A226" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="C226" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E216" s="2" t="s">
+      <c r="E226" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F216" s="2" t="s">
+      <c r="F226" s="2" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
content > show "preview" in stead of "preview and embed" in panels and drilldown
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@53938 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="326">
   <si>
     <t>Dashboard</t>
   </si>
@@ -991,6 +991,9 @@
   </si>
   <si>
     <t>customDataDrilldown.</t>
+  </si>
+  <si>
+    <t>showEmbedCode</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1382,8 @@
   <dimension ref="A1:G226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79:D86"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2205,7 +2208,7 @@
         <v>303</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f t="shared" ref="D74:D86" si="5">CONCATENATE($C$72,C74)</f>
+        <f t="shared" ref="D74:D76" si="5">CONCATENATE($C$72,C74)</f>
         <v>account.metadata.actionBox</v>
       </c>
     </row>
@@ -2980,6 +2983,12 @@
       </c>
       <c r="C140" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="141" spans="1:6">

</xml_diff>

<commit_message>
conversion profile popup mapping and some refactoring
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54022 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="346">
   <si>
     <t>Dashboard</t>
   </si>
@@ -147,24 +147,12 @@
     <t>deleteProfilesBtn</t>
   </si>
   <si>
-    <t>account.transcoding</t>
-  </si>
-  <si>
     <t>transcoding settings</t>
   </si>
   <si>
     <t>transcoding table</t>
   </si>
   <si>
-    <t xml:space="preserve">advance/simple mode button </t>
-  </si>
-  <si>
-    <t>conversionSettingsTable1</t>
-  </si>
-  <si>
-    <t>switchModeBtn</t>
-  </si>
-  <si>
     <t>saveButton</t>
   </si>
   <si>
@@ -994,6 +982,78 @@
   </si>
   <si>
     <t>showEmbedCode</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>content.generalPermissions</t>
+  </si>
+  <si>
+    <t>account.transcoding.</t>
+  </si>
+  <si>
+    <t>viewStack</t>
+  </si>
+  <si>
+    <t>contents view stack</t>
+  </si>
+  <si>
+    <t>ViewStack</t>
+  </si>
+  <si>
+    <t>simpleTable</t>
+  </si>
+  <si>
+    <t>advancedModeBtn</t>
+  </si>
+  <si>
+    <t>to advanced mode</t>
+  </si>
+  <si>
+    <t>to simple mode</t>
+  </si>
+  <si>
+    <t>simpleModeBtn</t>
+  </si>
+  <si>
+    <t>conversionProfilesTable</t>
+  </si>
+  <si>
+    <t>conversion profiles table</t>
+  </si>
+  <si>
+    <t>deleteProfileBtn</t>
+  </si>
+  <si>
+    <t>container for actions box</t>
+  </si>
+  <si>
+    <t>addNewProfileBtn</t>
+  </si>
+  <si>
+    <t>add new profile</t>
+  </si>
+  <si>
+    <t>dataEditable</t>
+  </si>
+  <si>
+    <t>conversion profile drilldown</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>conversionProfileDrilldown.</t>
+  </si>
+  <si>
+    <t>conversionNameTextInput</t>
+  </si>
+  <si>
+    <t>conversionDescTextArea</t>
+  </si>
+  <si>
+    <t>flavorsTable</t>
   </si>
 </sst>
 </file>
@@ -1379,11 +1439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G226"/>
+  <dimension ref="A1:G239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F140" sqref="F140"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1412,10 +1472,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -1530,7 +1590,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>CONCATENATE($C$16,C17)</f>
@@ -1539,13 +1599,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>CONCATENATE($C$16,C18)</f>
@@ -1560,7 +1620,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" ref="D19" si="1">CONCATENATE($C$16,C19)</f>
@@ -1569,13 +1629,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D20" s="2" t="str">
         <f>CONCATENATE($C$16,C20)</f>
@@ -1587,13 +1647,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1658,13 +1718,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>CONCATENATE($C$22,C27)</f>
@@ -1711,13 +1771,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D33" s="2" t="str">
         <f>CONCATENATE($C$31,C33)</f>
@@ -1756,27 +1816,27 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D38" s="2" t="str">
         <f t="shared" ref="D38:D59" si="3">CONCATENATE($C$37,C38)</f>
@@ -1785,13 +1845,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D39" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1800,10 +1860,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="B40" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D40" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1812,10 +1872,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="B41" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D41" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1824,13 +1884,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D42" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1839,13 +1899,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D43" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1854,13 +1914,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D44" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1869,10 +1929,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="B45" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D45" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1881,13 +1941,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D46" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1896,13 +1956,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D47" s="2" t="str">
         <f t="shared" si="3"/>
@@ -1911,2141 +1971,2320 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D48" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.removeUnauthorisedBtn</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:6">
       <c r="B49" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D49" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.allCountriesRaddioBtn</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="B50" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D50" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.approvedCountiesRadioBtn</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:6">
       <c r="B51" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D51" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.approvedCountriesList</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:6">
       <c r="B52" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D52" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.addRemoveCountriesBtn</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:6">
       <c r="B53" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D53" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedCountriesRadioBtn</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6">
       <c r="B54" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D54" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.notApprovedCountriesList</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:6">
       <c r="B55" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D55" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.restrictCountriesLinkButton</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D56" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.secureKSCBBtn</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D57" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.freePerviewCBBtn</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D58" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.freePreviewDuration</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D59" s="2" t="str">
         <f t="shared" si="3"/>
         <v>acDrilldown.submitBtn</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:6">
       <c r="A61" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>32</v>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>327</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>47</v>
+        <v>325</v>
       </c>
       <c r="D62" s="2" t="str">
         <f>CONCATENATE($C$61,C62)</f>
-        <v>account.transcodingconversionSettingsTable1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>account.transcoding.viewStack</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D63" s="2" t="str">
+        <f>CONCATENATE($C$61,C63)</f>
+        <v>account.transcoding.simpleTable</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D64" s="2" t="str">
+        <f>CONCATENATE($C$61,C64)</f>
+        <v>account.transcoding.advancedModeBtn</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D63" s="2" t="str">
-        <f t="shared" ref="D63:D64" si="4">CONCATENATE($C$61,C63)</f>
-        <v>account.transcodingswitchModeBtn</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>account.transcodingsaveButton</v>
+      <c r="C65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="2" t="str">
+        <f t="shared" ref="D65" si="4">CONCATENATE($C$61,C65)</f>
+        <v>account.transcoding.saveButton</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D66" s="2" t="str">
+        <f t="shared" ref="D66:D77" si="5">CONCATENATE($C$61,C66)</f>
+        <v>account.transcoding.simpleModeBtn</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="5" t="s">
-        <v>51</v>
+      <c r="A67" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>54</v>
+        <v>333</v>
+      </c>
+      <c r="D67" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>account.transcoding.conversionProfilesTable</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="2" t="s">
-        <v>53</v>
+      <c r="A68" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>32</v>
+        <v>207</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>52</v>
+        <v>335</v>
       </c>
       <c r="D68" s="2" t="str">
-        <f>CONCATENATE($C$67,C68)</f>
-        <v>account.upgrade.customFieldsTable</v>
+        <f t="shared" si="5"/>
+        <v>account.transcoding.deleteProfileBtn</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>22</v>
+      <c r="A69" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>55</v>
+        <v>299</v>
       </c>
       <c r="D69" s="2" t="str">
-        <f>CONCATENATE($C$67,C69)</f>
-        <v>account.upgrade.addFieldButton</v>
+        <f t="shared" si="5"/>
+        <v>account.transcoding.actionBox</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="2" t="s">
-        <v>57</v>
+      <c r="A70" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>56</v>
+        <v>337</v>
       </c>
       <c r="D70" s="2" t="str">
-        <f>CONCATENATE($C$67,C70)</f>
-        <v>account.upgrade.deleteCustomDataField</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>account.transcoding.addNewProfileBtn</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="4"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="5" t="s">
-        <v>304</v>
+      <c r="A72" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>306</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="4" t="s">
-        <v>305</v>
-      </c>
+      <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>56</v>
+        <v>343</v>
       </c>
       <c r="D73" s="2" t="str">
         <f>CONCATENATE($C$72,C73)</f>
-        <v>account.metadata.deleteCustomDataField</v>
+        <v>conversionProfileDrilldown.conversionNameTextInput</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>6</v>
+      <c r="A74" s="4"/>
+      <c r="B74" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f t="shared" ref="D74:D76" si="5">CONCATENATE($C$72,C74)</f>
-        <v>account.metadata.actionBox</v>
+        <f t="shared" ref="D74:D77" si="6">CONCATENATE($C$72,C74)</f>
+        <v>conversionProfileDrilldown.conversionDescTextArea</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>211</v>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>55</v>
+        <v>345</v>
       </c>
       <c r="D75" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>account.metadata.addFieldButton</v>
+        <f t="shared" si="6"/>
+        <v>conversionProfileDrilldown.flavorsTable</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>32</v>
+      <c r="A76" s="4"/>
+      <c r="B76" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>52</v>
+        <v>167</v>
       </c>
       <c r="D76" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>account.metadata.customFieldsTable</v>
+        <f t="shared" si="6"/>
+        <v>conversionProfileDrilldown.submitBtn</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="4" t="s">
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="2" t="str">
+        <f>CONCATENATE($C$79,C80)</f>
+        <v>account.upgrade.customFieldsTable</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D81" s="2" t="str">
+        <f>CONCATENATE($C$79,C81)</f>
+        <v>account.upgrade.addFieldButton</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="2" t="str">
+        <f>CONCATENATE($C$79,C82)</f>
+        <v>account.upgrade.deleteCustomDataField</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D85" s="2" t="str">
+        <f>CONCATENATE($C$84,C85)</f>
+        <v>account.metadata.deleteCustomDataField</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D86" s="2" t="str">
+        <f t="shared" ref="D86:D88" si="7">CONCATENATE($C$84,C86)</f>
+        <v>account.metadata.actionBox</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D87" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>account.metadata.addFieldButton</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>account.metadata.customFieldsTable</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D91" s="2" t="str">
+        <f>CONCATENATE($C$90,C91)</f>
+        <v>customDataDrilldown.saveBtn</v>
+      </c>
+      <c r="F91" s="4"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D92" s="2" t="str">
+        <f t="shared" ref="D92:D98" si="8">CONCATENATE($C$90,C92)</f>
+        <v>customDataDrilldown.fullDescriptionInput</v>
+      </c>
+      <c r="F92" s="4"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D93" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.descriptionInput</v>
+      </c>
+      <c r="F93" s="4"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="4"/>
+      <c r="B94" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D94" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.appearInSearchList</v>
+      </c>
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="4"/>
+      <c r="B95" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D79" s="2" t="str">
-        <f>CONCATENATE($C$78,C79)</f>
-        <v>customDataDrilldown.saveBtn</v>
-      </c>
-      <c r="F79" s="4"/>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="D95" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.maxValuesList</v>
+      </c>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D80" s="2" t="str">
-        <f t="shared" ref="D80:D86" si="6">CONCATENATE($C$78,C80)</f>
-        <v>customDataDrilldown.fullDescriptionInput</v>
-      </c>
-      <c r="F80" s="4"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="D96" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.optionalValuesInput</v>
+      </c>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="1:7" ht="12" customHeight="1">
+      <c r="A97" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D81" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>customDataDrilldown.descriptionInput</v>
-      </c>
-      <c r="F81" s="4"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="4"/>
-      <c r="B82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D82" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>customDataDrilldown.appearInSearchList</v>
-      </c>
-      <c r="F82" s="4"/>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="4"/>
-      <c r="B83" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D83" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>customDataDrilldown.maxValuesList</v>
-      </c>
-      <c r="F83" s="4"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D84" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>customDataDrilldown.optionalValuesInput</v>
-      </c>
-      <c r="F84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" ht="12" customHeight="1">
-      <c r="A85" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D85" s="2" t="str">
-        <f t="shared" si="6"/>
+      <c r="D97" s="2" t="str">
+        <f t="shared" si="8"/>
         <v>customDataDrilldown.fieldTypeList</v>
       </c>
-      <c r="F85" s="4"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D86" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>customDataDrilldown.fieldNameInput</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D90" s="2" t="str">
-        <f>CONCATENATE($C$89,C90)</f>
-        <v>admin.users.table</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D91" s="2" t="str">
-        <f>CONCATENATE($C$89,C91)</f>
-        <v>admin.users.addBtn</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D92" s="2" t="str">
-        <f>CONCATENATE($C$89,C92)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D93" s="2" t="str">
-        <f>CONCATENATE($C$89,C93)</f>
-        <v>admin.users.table</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D96" s="2" t="str">
-        <f>CONCATENATE($C$89,C96)</f>
-        <v>admin.users.table</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D97" s="2" t="str">
-        <f>CONCATENATE($C$89,C97)</f>
-        <v>admin.users.addBtn</v>
-      </c>
+      <c r="F97" s="4"/>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="2" t="s">
-        <v>68</v>
+        <v>315</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>67</v>
+        <v>314</v>
       </c>
       <c r="D98" s="2" t="str">
-        <f>CONCATENATE($C$89,C98)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C99" s="2" t="s">
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.fieldNameInput</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D99" s="2" t="str">
-        <f>CONCATENATE($C$89,C99)</f>
+      <c r="B102" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="2" t="str">
+        <f>CONCATENATE($C$101,C102)</f>
         <v>admin.users.table</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="7" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="5" t="s">
-        <v>72</v>
+      <c r="A103" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="D103" s="2" t="str">
+        <f>CONCATENATE($C$101,C103)</f>
+        <v>admin.users.addBtn</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D104" s="2" t="str">
+        <f>CONCATENATE($C$101,C104)</f>
+        <v>admin.users.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105" s="2" t="str">
+        <f>CONCATENATE($C$101,C105)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D104" s="2" t="str">
-        <f>CONCATENATE($C$103,C104)</f>
+      <c r="G105" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" s="2" t="str">
+        <f>CONCATENATE($C$101,C108)</f>
+        <v>admin.users.table</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D109" s="2" t="str">
+        <f>CONCATENATE($C$101,C109)</f>
+        <v>admin.users.addBtn</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D110" s="2" t="str">
+        <f>CONCATENATE($C$101,C110)</f>
+        <v>admin.users.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111" s="2" t="str">
+        <f>CONCATENATE($C$101,C111)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D116" s="2" t="str">
+        <f>CONCATENATE($C$115,C116)</f>
         <v>studio.playerList.templatesHolder</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G105" s="2" t="s">
+    <row r="117" spans="1:7">
+      <c r="A117" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D106" s="2" t="str">
-        <f>CONCATENATE($C$105,C106)</f>
+      <c r="B117" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D118" s="2" t="str">
+        <f>CONCATENATE($C$117,C118)</f>
         <v>wizard.wizardSaveBtn</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="1" t="s">
+    <row r="119" spans="1:7">
+      <c r="A119" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D119" s="1" t="str">
+        <f t="shared" ref="D119" si="9">CONCATENATE($C$117,C119)</f>
+        <v>wizard.templatePage.</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D120" s="1" t="str">
+        <f t="shared" ref="D120:D127" si="10">CONCATENATE($D$119,C120)</f>
+        <v>wizard.templatePage.all</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D121" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.playerName</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D122" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.keepOriginalRatio</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D107" s="1" t="str">
-        <f t="shared" ref="D107" si="7">CONCATENATE($C$105,C107)</f>
-        <v>wizard.templatePage.</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D108" s="1" t="str">
-        <f t="shared" ref="D108:D115" si="8">CONCATENATE($D$107,C108)</f>
-        <v>wizard.templatePage.all</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
-      <c r="A109" s="1" t="s">
+      <c r="D123" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.streachMediaToFitPlayer</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D124" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.templateAutoPlay</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D109" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.playerName</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" s="1" t="s">
+      <c r="D125" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.templateAutoMute</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D110" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.keepOriginalRatio</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D111" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.streachMediaToFitPlayer</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B112" s="1" t="s">
+      <c r="D126" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.playlistAutoContinue</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D112" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.templateAutoPlay</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D113" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.templateAutoMute</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D114" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>wizard.templatePage.playlistAutoContinue</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D115" s="1" t="str">
-        <f t="shared" si="8"/>
+      <c r="D127" s="1" t="str">
+        <f t="shared" si="10"/>
         <v>wizard.templatePage.playlistImagesInterval</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D117" s="2" t="str">
-        <f>CONCATENATE($C$105,C117)</f>
-        <v>wizard.featurePage.</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D118" s="2" t="str">
-        <f>CONCATENATE($D$117,C118)</f>
-        <v>wizard.featurePage.accordi</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D119" s="2" t="str">
-        <f>CONCATENATE($D$117,C119)</f>
-        <v>wizard.featurePage.featureScreen</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D120" s="2" t="str">
-        <f>CONCATENATE($D$117,C120)</f>
-        <v>wizard.featurePage.keyValueBox</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D122" s="2" t="str">
-        <f>CONCATENATE($C$105,C122)</f>
-        <v>wizard.advertizingPage</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D124" s="2" t="str">
-        <f>CONCATENATE($C$105,C124)</f>
-        <v>wizard.stylePage</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D126" s="2" t="str">
-        <f>CONCATENATE($C$105,C126)</f>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D127" s="2" t="str">
-        <f>CONCATENATE($D$126,C127)</f>
-        <v>wizard.contentPage.all</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="D129" s="2" t="str">
-        <f>CONCATENATE($C$105,C129)</f>
-        <v>wizard.previewPlayerPage.</v>
+        <f>CONCATENATE($C$117,C129)</f>
+        <v>wizard.featurePage.</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="D130" s="2" t="str">
-        <f t="shared" ref="D130:D135" si="9">CONCATENATE($D$129,C130)</f>
-        <v>wizard.previewPlayerPage.controls</v>
+        <f>CONCATENATE($D$129,C130)</f>
+        <v>wizard.featurePage.accordi</v>
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="2" t="s">
-        <v>239</v>
+      <c r="A131" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>211</v>
+        <v>6</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D131" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>wizard.previewPlayerPage.openClosePreview</v>
+        <f>CONCATENATE($D$129,C131)</f>
+        <v>wizard.featurePage.featureScreen</v>
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>233</v>
+      <c r="A132" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D132" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>wizard.previewPlayerPage.kdpWidth</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D133" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>wizard.previewPlayerPage.kdpHeight</v>
+        <f>CONCATENATE($D$129,C132)</f>
+        <v>wizard.featurePage.keyValueBox</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="2" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>211</v>
+        <v>6</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>243</v>
+        <v>83</v>
       </c>
       <c r="D134" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>wizard.previewPlayerPage.refreshKdp3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="2" t="s">
+        <f>CONCATENATE($C$117,C134)</f>
+        <v>wizard.advertizingPage</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D136" s="2" t="str">
+        <f>CONCATENATE($C$117,C136)</f>
+        <v>wizard.stylePage</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D138" s="2" t="str">
+        <f>CONCATENATE($C$117,C138)</f>
+        <v>wizard.contentPage.</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D135" s="2" t="str">
-        <f t="shared" si="9"/>
-        <v>wizard.previewPlayerPage.autoPreview</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="F140" s="4" t="s">
-        <v>99</v>
+      <c r="D139" s="2" t="str">
+        <f>CONCATENATE($D$138,C139)</f>
+        <v>wizard.contentPage.all</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" s="2" t="s">
-        <v>91</v>
+        <v>215</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>92</v>
+        <v>236</v>
       </c>
       <c r="D141" s="2" t="str">
-        <f>CONCATENATE($C$140,C141)</f>
-        <v>content.manage.entryTable</v>
+        <f>CONCATENATE($C$117,C141)</f>
+        <v>wizard.previewPlayerPage.</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D142" s="2" t="str">
+        <f t="shared" ref="D142:D147" si="11">CONCATENATE($D$141,C142)</f>
+        <v>wizard.previewPlayerPage.controls</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
-        <v>94</v>
+        <v>235</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="D143" s="2" t="str">
-        <f>CONCATENATE($C$140,C143)</f>
-        <v>content.manage.toolBar.</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>99</v>
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.openClosePreview</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="2" t="s">
-        <v>95</v>
+        <v>241</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>97</v>
+        <v>237</v>
       </c>
       <c r="D144" s="2" t="str">
-        <f>CONCATENATE($D$143,C144)</f>
-        <v>content.manage.toolBar.deleteBtn</v>
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.kdpWidth</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="2" t="s">
-        <v>96</v>
+        <v>242</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>110</v>
+        <v>238</v>
       </c>
       <c r="D145" s="2" t="str">
-        <f t="shared" ref="D145:D149" si="10">CONCATENATE($D$143,C145)</f>
-        <v>content.manage.toolBar.newStreamBtn</v>
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.kdpHeight</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="D146" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.toolBar.download</v>
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.refreshKdp3</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" s="2" t="s">
-        <v>105</v>
+        <v>244</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>104</v>
+        <v>225</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>103</v>
+        <v>240</v>
       </c>
       <c r="D147" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.toolBar.tagsCombo</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D148" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.toolBar.playlistCombo</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D149" s="2" t="str">
-        <f t="shared" si="10"/>
-        <v>content.manage.toolBar.moreOption</v>
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.autoPreview</v>
       </c>
     </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D151" s="2" t="str">
-        <f>CONCATENATE($C$140,C151)</f>
-        <v>content.manage.filter.</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>99</v>
+      <c r="A151" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>6</v>
+        <v>322</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D152" s="2" t="str">
-        <f>CONCATENATE($D$151,C152)</f>
-        <v>content.manage.filter.searchBox</v>
+        <v>323</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="153" spans="1:6">
-      <c r="A153" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>6</v>
+      <c r="A153" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D153" s="2" t="str">
-        <f t="shared" ref="D153:D161" si="11">CONCATENATE($D$151,C153)</f>
-        <v>content.manage.filter.dateCont</v>
+        <v>86</v>
       </c>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" s="2" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="D154" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.mediaTypes</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D155" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.conversionStatus</v>
+        <f>CONCATENATE($C$153,C154)</f>
+        <v>content.manage.entryTable</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.durationStatus</v>
+        <f>CONCATENATE($C$153,C156)</f>
+        <v>content.manage.toolBar.</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="2" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.scheduling</v>
+        <f>CONCATENATE($D$156,C157)</f>
+        <v>content.manage.toolBar.deleteBtn</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="2" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.moderationStatus</v>
+        <f t="shared" ref="D158:D162" si="12">CONCATENATE($D$156,C158)</f>
+        <v>content.manage.toolBar.newStreamBtn</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="2" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="D159" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.accessControl</v>
+        <f t="shared" si="12"/>
+        <v>content.manage.toolBar.download</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="D160" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.transcodingFlavor</v>
+        <f t="shared" si="12"/>
+        <v>content.manage.toolBar.tagsCombo</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="D161" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>content.manage.filter.categoriesBox</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>136</v>
+        <f t="shared" si="12"/>
+        <v>content.manage.toolBar.playlistCombo</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D162" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>content.manage.toolBar.moreOption</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>CONCATENATE($C$163,C164)</f>
-        <v>content.moderation.filter.</v>
+        <f>CONCATENATE($C$153,C164)</f>
+        <v>content.manage.filter.</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>CONCATENATE($D$151,C165)</f>
+        <f>CONCATENATE($D$164,C165)</f>
         <v>content.manage.filter.searchBox</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f t="shared" ref="D166:D174" si="12">CONCATENATE($D$151,C166)</f>
+        <f t="shared" ref="D166:D174" si="13">CONCATENATE($D$164,C166)</f>
         <v>content.manage.filter.dateCont</v>
       </c>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.mediaTypes</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D168" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.conversionStatus</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.durationStatus</v>
       </c>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.scheduling</v>
       </c>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.moderationStatus</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.accessControl</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D173" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>content.manage.filter.transcodingFlavor</v>
       </c>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D174" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>content.manage.filter.categoriesBox</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D177" s="2" t="str">
+        <f>CONCATENATE($C$176,C177)</f>
+        <v>content.moderation.filter.</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D178" s="2" t="str">
+        <f>CONCATENATE($D$164,C178)</f>
+        <v>content.manage.filter.searchBox</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D179" s="2" t="str">
+        <f t="shared" ref="D179:D187" si="14">CONCATENATE($D$164,C179)</f>
+        <v>content.manage.filter.dateCont</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D180" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.mediaTypes</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D181" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.conversionStatus</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D182" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D183" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.scheduling</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D184" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.moderationStatus</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D185" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.accessControl</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D186" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D187" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.categoriesBox</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D189" s="2" t="str">
+        <f>CONCATENATE($C$176,C189)</f>
+        <v>content.moderation.entryTable</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D190" s="2" t="str">
+        <f>CONCATENATE($C$176,C190)</f>
+        <v>content.moderation.toolBar.</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D174" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>content.manage.filter.categoriesBox</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
-      <c r="A176" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D176" s="2" t="str">
-        <f>CONCATENATE($C$163,C176)</f>
-        <v>content.moderation.entryTable</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D177" s="2" t="str">
-        <f>CONCATENATE($C$163,C177)</f>
-        <v>content.moderation.toolBar.</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D178" s="2" t="str">
-        <f>CONCATENATE($D$177,C178)</f>
-        <v>content.moderation.toolBar.approveSelected</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D179" s="2" t="str">
-        <f>CONCATENATE($D$177,C179)</f>
-        <v>content.moderation.toolBar.rejectSelected</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
-      <c r="A181" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
-      <c r="A182" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D182" s="2" t="str">
-        <f>CONCATENATE($C$181,C182)</f>
-        <v>content.playlists.filter</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="A183" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D183" s="2" t="str">
-        <f>CONCATENATE($D$182,C183)</f>
-        <v>content.playlists.filterfreeText</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="A184" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D184" s="2" t="str">
-        <f>CONCATENATE($D$182,C184)</f>
-        <v>content.playlists.filterdateCont</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
-      <c r="A186" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D186" s="2" t="str">
-        <f t="shared" ref="D186:D192" si="13">CONCATENATE($C$181,C186)</f>
-        <v>content.playlists.entryTableContainer</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
-      <c r="A187" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D187" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.playlists.toolBar.</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D188" s="2" t="str">
-        <f>CONCATENATE($D$187,C188)</f>
-        <v>content.playlists.toolBar.deleteBtn</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
-      <c r="A190" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D190" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.playlists.actionsBox</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.playlists.addManualPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
+        <f>CONCATENATE($D$190,C191)</f>
+        <v>content.moderation.toolBar.approveSelected</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D192" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.playlists.addRuleBasedPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6">
+        <f>CONCATENATE($D$190,C192)</f>
+        <v>content.moderation.toolBar.rejectSelected</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
       <c r="A194" s="5" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" s="2" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="D195" s="2" t="str">
         <f>CONCATENATE($C$194,C195)</f>
-        <v>content.syndication.feedsTable</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6">
+        <v>content.playlists.filter</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196" s="2" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="B196" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D196" s="2" t="str">
+        <f>CONCATENATE($D$195,C196)</f>
+        <v>content.playlists.filterfreeText</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D197" s="2" t="str">
+        <f>CONCATENATE($D$195,C197)</f>
+        <v>content.playlists.filterdateCont</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D199" s="2" t="str">
+        <f t="shared" ref="D199:D205" si="15">CONCATENATE($C$194,C199)</f>
+        <v>content.playlists.entryTableContainer</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D200" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.playlists.toolBar.</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D196" s="2" t="str">
-        <f>CONCATENATE($C$194,C196)</f>
-        <v>content.syndication.deleteExSynBtn</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6">
-      <c r="A197" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C197" s="2" t="s">
+      <c r="C201" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D201" s="2" t="str">
+        <f>CONCATENATE($D$200,C201)</f>
+        <v>content.playlists.toolBar.deleteBtn</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D203" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.playlists.actionsBox</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D204" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.playlists.addManualPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="D197" s="2" t="str">
-        <f t="shared" ref="D197:D198" si="14">CONCATENATE($C$194,C197)</f>
-        <v>content.syndication.actionsBox</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6">
-      <c r="A198" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D198" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.syndication.addBtn</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6">
-      <c r="A200" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E200" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F200" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6">
-      <c r="A202" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6">
-      <c r="A203" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D203" s="2" t="str">
-        <f>CONCATENATE($C$202,C203)</f>
-        <v>content.upload.kcwBox</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6">
-      <c r="A204" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D204" s="2" t="str">
-        <f t="shared" ref="D204:D205" si="15">CONCATENATE($C$202,C204)</f>
-        <v>content.upload.profilesCb</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6">
-      <c r="A205" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D205" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>content.upload.kcwBtn</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6">
-      <c r="A206" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D206" s="2" t="str">
-        <f t="shared" ref="D206:D207" si="16">CONCATENATE($C$202,C206)</f>
-        <v>content.upload.bulkUploadBox</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6">
-      <c r="A207" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B207" s="2" t="s">
+        <v>content.playlists.addRuleBasedPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D208" s="2" t="str">
+        <f>CONCATENATE($C$207,C208)</f>
+        <v>content.syndication.feedsTable</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7">
+      <c r="A209" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C207" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D207" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>content.upload.submitBtn</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="A209" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="C209" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E209" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G209" s="2" t="s">
-        <v>80</v>
+        <v>150</v>
+      </c>
+      <c r="D209" s="2" t="str">
+        <f>CONCATENATE($C$207,C209)</f>
+        <v>content.syndication.deleteExSynBtn</v>
       </c>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="2" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f>CONCATENATE($C$209,C210)</f>
-        <v>entryDrilldown.entryMetaData.</v>
+        <f t="shared" ref="D210:D211" si="16">CONCATENATE($C$207,C210)</f>
+        <v>content.syndication.actionsBox</v>
       </c>
     </row>
     <row r="211" spans="1:7">
       <c r="A211" s="2" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>174</v>
+        <v>22</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="D211" s="2" t="str">
-        <f>CONCATENATE($D$210,C211)</f>
-        <v>entryDrilldown.entryMetaData.name_input</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7">
-      <c r="A212" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D212" s="2" t="str">
-        <f t="shared" ref="D212:D215" si="17">CONCATENATE($D$210,C212)</f>
-        <v>entryDrilldown.entryMetaData.descriptionTi</v>
+        <f t="shared" si="16"/>
+        <v>content.syndication.addBtn</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>174</v>
+      <c r="A213" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D213" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v>entryDrilldown.entryMetaData.tagsTi</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7">
-      <c r="A214" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D214" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
+        <v>169</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>6</v>
+      <c r="A215" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D215" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
+      <c r="A216" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D216" s="2" t="str">
+        <f>CONCATENATE($C$215,C216)</f>
+        <v>content.upload.kcwBox</v>
       </c>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="2" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f>CONCATENATE($C$209,C217)</f>
-        <v>entryDrilldown.entryAcp.</v>
+        <f t="shared" ref="D217:D218" si="17">CONCATENATE($C$215,C217)</f>
+        <v>content.upload.profilesCb</v>
       </c>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="2" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>175</v>
+        <v>22</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f>CONCATENATE($D$217,C218)</f>
-        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+        <f t="shared" si="17"/>
+        <v>content.upload.kcwBtn</v>
       </c>
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>65</v>
+        <v>158</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f>CONCATENATE($D$217,C219)</f>
-        <v>entryDrilldown.entryAcp.addBtn</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7">
-      <c r="A221" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D221" s="2" t="str">
-        <f>CONCATENATE($C$209,C221)</f>
-        <v>entryDrilldown.customData</v>
+        <f t="shared" ref="D219:D220" si="18">CONCATENATE($C$215,C219)</f>
+        <v>content.upload.bulkUploadBox</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D220" s="2" t="str">
+        <f t="shared" si="18"/>
+        <v>content.upload.submitBtn</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G222" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="223" spans="1:7">
       <c r="A223" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D223" s="2" t="str">
+        <f>CONCATENATE($C$222,C223)</f>
+        <v>entryDrilldown.entryMetaData.</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D224" s="2" t="str">
+        <f>CONCATENATE($D$223,C224)</f>
+        <v>entryDrilldown.entryMetaData.name_input</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
+      <c r="A225" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D225" s="2" t="str">
+        <f t="shared" ref="D225:D228" si="19">CONCATENATE($D$223,C225)</f>
+        <v>entryDrilldown.entryMetaData.descriptionTi</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7">
+      <c r="A226" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D226" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>entryDrilldown.entryMetaData.tagsTi</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7">
+      <c r="A227" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D227" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7">
+      <c r="A228" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D228" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D230" s="2" t="str">
+        <f>CONCATENATE($C$222,C230)</f>
+        <v>entryDrilldown.entryAcp.</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
+      <c r="A231" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D231" s="2" t="str">
+        <f>CONCATENATE($D$230,C231)</f>
+        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="A232" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D232" s="2" t="str">
+        <f>CONCATENATE($D$230,C232)</f>
+        <v>entryDrilldown.entryAcp.addBtn</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D234" s="2" t="str">
+        <f>CONCATENATE($C$222,C234)</f>
+        <v>entryDrilldown.customData</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
+      <c r="A236" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D236" s="2" t="str">
+        <f>CONCATENATE($C$222,C236)</f>
+        <v>entryDrilldown.entryAsstes</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F236" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G236" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B223" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C223" s="2" t="s">
+      <c r="C238" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D223" s="2" t="str">
-        <f>CONCATENATE($C$209,C223)</f>
-        <v>entryDrilldown.entryAsstes</v>
-      </c>
-      <c r="E223" s="2" t="s">
+      <c r="E238" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F223" s="2" t="s">
+      <c r="F238" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="G223" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="8" t="s">
+      <c r="C239" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C225" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E225" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F225" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E226" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F226" s="2" t="s">
-        <v>99</v>
+      <c r="E239" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entry drilldown > scheduling mapping
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54023 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="359">
   <si>
     <t>Dashboard</t>
   </si>
@@ -1054,6 +1054,45 @@
   </si>
   <si>
     <t>flavorsTable</t>
+  </si>
+  <si>
+    <t>flavors list</t>
+  </si>
+  <si>
+    <t>scheduling panel</t>
+  </si>
+  <si>
+    <t>entrySch.</t>
+  </si>
+  <si>
+    <t>anyTimeRBtn</t>
+  </si>
+  <si>
+    <t>spcificRangeRBtn</t>
+  </si>
+  <si>
+    <t>sepcificStartDate</t>
+  </si>
+  <si>
+    <t>DateField</t>
+  </si>
+  <si>
+    <t>sepcificStartHour</t>
+  </si>
+  <si>
+    <t>specificEndCBBtn</t>
+  </si>
+  <si>
+    <t>specificEndDate</t>
+  </si>
+  <si>
+    <t>specificEndHour</t>
+  </si>
+  <si>
+    <t>clearDatesBtn</t>
+  </si>
+  <si>
+    <t>only handles the things that are otherwise bound</t>
   </si>
 </sst>
 </file>
@@ -1439,11 +1478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G239"/>
+  <dimension ref="A1:G248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D230" sqref="D230:D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2213,7 +2252,7 @@
         <v>332</v>
       </c>
       <c r="D66" s="2" t="str">
-        <f t="shared" ref="D66:D77" si="5">CONCATENATE($C$61,C66)</f>
+        <f t="shared" ref="D66:D70" si="5">CONCATENATE($C$61,C66)</f>
         <v>account.transcoding.simpleModeBtn</v>
       </c>
     </row>
@@ -2292,7 +2331,9 @@
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="4"/>
+      <c r="A73" s="4" t="s">
+        <v>266</v>
+      </c>
       <c r="B73" s="2" t="s">
         <v>170</v>
       </c>
@@ -2305,7 +2346,9 @@
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="4"/>
+      <c r="A74" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="B74" s="2" t="s">
         <v>180</v>
       </c>
@@ -2313,12 +2356,14 @@
         <v>344</v>
       </c>
       <c r="D74" s="2" t="str">
-        <f t="shared" ref="D74:D77" si="6">CONCATENATE($C$72,C74)</f>
+        <f t="shared" ref="D74:D76" si="6">CONCATENATE($C$72,C74)</f>
         <v>conversionProfileDrilldown.conversionDescTextArea</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="4"/>
+      <c r="A75" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="B75" s="4" t="s">
         <v>32</v>
       </c>
@@ -2337,7 +2382,9 @@
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="B76" s="2" t="s">
         <v>207</v>
       </c>
@@ -2349,194 +2396,205 @@
         <v>conversionProfileDrilldown.submitBtn</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="4"/>
+    <row r="78" spans="1:6">
+      <c r="A78" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="5" t="s">
-        <v>47</v>
+      <c r="A79" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="D79" s="2" t="str">
+        <f>CONCATENATE($C$78,C79)</f>
+        <v>account.upgrade.customFieldsTable</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D80" s="2" t="str">
-        <f>CONCATENATE($C$79,C80)</f>
-        <v>account.upgrade.customFieldsTable</v>
+        <f>CONCATENATE($C$78,C80)</f>
+        <v>account.upgrade.addFieldButton</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D81" s="2" t="str">
-        <f>CONCATENATE($C$79,C81)</f>
-        <v>account.upgrade.addFieldButton</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C82" s="2" t="s">
+        <f>CONCATENATE($C$78,C81)</f>
+        <v>account.upgrade.deleteCustomDataField</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="2" t="str">
-        <f>CONCATENATE($C$79,C82)</f>
-        <v>account.upgrade.deleteCustomDataField</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>302</v>
+      <c r="D84" s="2" t="str">
+        <f>CONCATENATE($C$83,C84)</f>
+        <v>account.metadata.deleteCustomDataField</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>207</v>
+        <v>303</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>52</v>
+        <v>299</v>
       </c>
       <c r="D85" s="2" t="str">
-        <f>CONCATENATE($C$84,C85)</f>
-        <v>account.metadata.deleteCustomDataField</v>
+        <f t="shared" ref="D85:D87" si="7">CONCATENATE($C$83,C85)</f>
+        <v>account.metadata.actionBox</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>6</v>
+        <v>304</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>299</v>
+        <v>51</v>
       </c>
       <c r="D86" s="2" t="str">
-        <f t="shared" ref="D86:D88" si="7">CONCATENATE($C$84,C86)</f>
-        <v>account.metadata.actionBox</v>
+        <f t="shared" si="7"/>
+        <v>account.metadata.addFieldButton</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>207</v>
+        <v>305</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D87" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>account.metadata.addFieldButton</v>
+        <v>account.metadata.customFieldsTable</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D88" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>account.metadata.customFieldsTable</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="4"/>
+      <c r="A89" s="4" t="s">
+        <v>307</v>
+      </c>
       <c r="B89" s="4"/>
+      <c r="C89" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B90" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="C90" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>95</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D90" s="2" t="str">
+        <f>CONCATENATE($C$89,C90)</f>
+        <v>customDataDrilldown.saveBtn</v>
+      </c>
+      <c r="F90" s="4"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="4" t="s">
-        <v>46</v>
+        <v>319</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="D91" s="2" t="str">
-        <f>CONCATENATE($C$90,C91)</f>
-        <v>customDataDrilldown.saveBtn</v>
+        <f t="shared" ref="D91:D97" si="8">CONCATENATE($C$89,C91)</f>
+        <v>customDataDrilldown.fullDescriptionInput</v>
       </c>
       <c r="F91" s="4"/>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D92" s="2" t="str">
-        <f t="shared" ref="D92:D98" si="8">CONCATENATE($C$90,C92)</f>
-        <v>customDataDrilldown.fullDescriptionInput</v>
+        <f t="shared" si="8"/>
+        <v>customDataDrilldown.descriptionInput</v>
       </c>
       <c r="F92" s="4"/>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="4" t="s">
-        <v>318</v>
-      </c>
+      <c r="A93" s="4"/>
       <c r="B93" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D93" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>customDataDrilldown.descriptionInput</v>
+        <v>customDataDrilldown.appearInSearchList</v>
       </c>
       <c r="F93" s="4"/>
     </row>
@@ -2546,340 +2604,341 @@
         <v>171</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D94" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>customDataDrilldown.appearInSearchList</v>
+        <v>customDataDrilldown.maxValuesList</v>
       </c>
       <c r="F94" s="4"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="4"/>
+      <c r="A95" s="4" t="s">
+        <v>317</v>
+      </c>
       <c r="B95" s="2" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D95" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>customDataDrilldown.maxValuesList</v>
+        <v>customDataDrilldown.optionalValuesInput</v>
       </c>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" ht="12" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D96" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>customDataDrilldown.optionalValuesInput</v>
+        <v>customDataDrilldown.fieldTypeList</v>
       </c>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="1:7" ht="12" customHeight="1">
-      <c r="A97" s="4" t="s">
-        <v>316</v>
+    <row r="97" spans="1:7">
+      <c r="A97" s="2" t="s">
+        <v>315</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D97" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>customDataDrilldown.fieldTypeList</v>
-      </c>
-      <c r="F97" s="4"/>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D98" s="2" t="str">
-        <f t="shared" si="8"/>
         <v>customDataDrilldown.fieldNameInput</v>
       </c>
     </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="7" t="s">
-        <v>58</v>
+      <c r="A100" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="5" t="s">
-        <v>59</v>
+      <c r="A101" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="D101" s="2" t="str">
+        <f>CONCATENATE($C$100,C101)</f>
+        <v>admin.users.table</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D102" s="2" t="str">
-        <f>CONCATENATE($C$101,C102)</f>
-        <v>admin.users.table</v>
+        <f>CONCATENATE($C$100,C102)</f>
+        <v>admin.users.addBtn</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D103" s="2" t="str">
-        <f>CONCATENATE($C$101,C103)</f>
-        <v>admin.users.addBtn</v>
+        <f>CONCATENATE($C$100,C103)</f>
+        <v>admin.users.actionButtonsContainer</v>
       </c>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>6</v>
+      <c r="A104" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D104" s="2" t="str">
-        <f>CONCATENATE($C$101,C104)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C105" s="2" t="s">
+        <f>CONCATENATE($C$100,C104)</f>
+        <v>admin.users.table</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D105" s="2" t="str">
-        <f>CONCATENATE($C$101,C105)</f>
+      <c r="B107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D107" s="2" t="str">
+        <f>CONCATENATE($C$100,C107)</f>
         <v>admin.users.table</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="2" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D108" s="2" t="str">
-        <f>CONCATENATE($C$101,C108)</f>
-        <v>admin.users.table</v>
+        <f>CONCATENATE($C$100,C108)</f>
+        <v>admin.users.addBtn</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D109" s="2" t="str">
-        <f>CONCATENATE($C$101,C109)</f>
-        <v>admin.users.addBtn</v>
+        <f>CONCATENATE($C$100,C109)</f>
+        <v>admin.users.actionButtonsContainer</v>
       </c>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>6</v>
+      <c r="A110" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D110" s="2" t="str">
-        <f>CONCATENATE($C$101,C110)</f>
-        <v>admin.users.actionButtonsContainer</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D111" s="2" t="str">
-        <f>CONCATENATE($C$101,C111)</f>
+        <f>CONCATENATE($C$100,C110)</f>
         <v>admin.users.table</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E110" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="114" spans="1:7">
-      <c r="A114" s="7" t="s">
-        <v>67</v>
+      <c r="A114" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:7">
-      <c r="A115" s="5" t="s">
-        <v>68</v>
+      <c r="A115" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="D115" s="2" t="str">
+        <f>CONCATENATE($C$114,C115)</f>
+        <v>studio.playerList.templatesHolder</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D116" s="2" t="str">
-        <f>CONCATENATE($C$115,C116)</f>
-        <v>studio.playerList.templatesHolder</v>
+        <v>209</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="2" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>81</v>
+        <v>207</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>76</v>
+        <v>206</v>
+      </c>
+      <c r="D117" s="2" t="str">
+        <f>CONCATENATE($C$116,C117)</f>
+        <v>wizard.wizardSaveBtn</v>
       </c>
     </row>
     <row r="118" spans="1:7">
-      <c r="A118" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D118" s="2" t="str">
-        <f>CONCATENATE($C$117,C118)</f>
-        <v>wizard.wizardSaveBtn</v>
+      <c r="A118" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D118" s="1" t="str">
+        <f t="shared" ref="D118" si="9">CONCATENATE($C$116,C118)</f>
+        <v>wizard.templatePage.</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="1" t="s">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
       <c r="D119" s="1" t="str">
-        <f t="shared" ref="D119" si="9">CONCATENATE($C$117,C119)</f>
-        <v>wizard.templatePage.</v>
+        <f t="shared" ref="D119:D126" si="10">CONCATENATE($D$118,C119)</f>
+        <v>wizard.templatePage.all</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="1" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="D120" s="1" t="str">
-        <f t="shared" ref="D120:D127" si="10">CONCATENATE($D$119,C120)</f>
-        <v>wizard.templatePage.all</v>
+        <f t="shared" si="10"/>
+        <v>wizard.templatePage.playerName</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>170</v>
+        <v>221</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D121" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.playerName</v>
+        <v>wizard.templatePage.keepOriginalRatio</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -2890,1400 +2949,1505 @@
         <v>221</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D122" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.keepOriginalRatio</v>
+        <v>wizard.templatePage.streachMediaToFitPlayer</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="1" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D123" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.streachMediaToFitPlayer</v>
+        <v>wizard.templatePage.templateAutoPlay</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D124" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.templateAutoPlay</v>
+        <v>wizard.templatePage.templateAutoMute</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>225</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D125" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.templateAutoMute</v>
+        <v>wizard.templatePage.playlistAutoContinue</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D126" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>wizard.templatePage.playlistAutoContinue</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B127" s="1" t="s">
+        <v>wizard.templatePage.playlistImagesInterval</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D128" s="2" t="str">
+        <f>CONCATENATE($C$116,C128)</f>
+        <v>wizard.featurePage.</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D129" s="2" t="str">
+        <f>CONCATENATE($D$128,C129)</f>
+        <v>wizard.featurePage.accordi</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D130" s="2" t="str">
+        <f>CONCATENATE($D$128,C130)</f>
+        <v>wizard.featurePage.featureScreen</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D131" s="2" t="str">
+        <f>CONCATENATE($D$128,C131)</f>
+        <v>wizard.featurePage.keyValueBox</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D133" s="2" t="str">
+        <f>CONCATENATE($C$116,C133)</f>
+        <v>wizard.advertizingPage</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D135" s="2" t="str">
+        <f>CONCATENATE($C$116,C135)</f>
+        <v>wizard.stylePage</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D137" s="2" t="str">
+        <f>CONCATENATE($C$116,C137)</f>
+        <v>wizard.contentPage.</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D138" s="2" t="str">
+        <f>CONCATENATE($D$137,C138)</f>
+        <v>wizard.contentPage.all</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D140" s="2" t="str">
+        <f>CONCATENATE($C$116,C140)</f>
+        <v>wizard.previewPlayerPage.</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D141" s="2" t="str">
+        <f t="shared" ref="D141:D146" si="11">CONCATENATE($D$140,C141)</f>
+        <v>wizard.previewPlayerPage.controls</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D142" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>wizard.previewPlayerPage.openClosePreview</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D127" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>wizard.templatePage.playlistImagesInterval</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D129" s="2" t="str">
-        <f>CONCATENATE($C$117,C129)</f>
-        <v>wizard.featurePage.</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D130" s="2" t="str">
-        <f>CONCATENATE($D$129,C130)</f>
-        <v>wizard.featurePage.accordi</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D131" s="2" t="str">
-        <f>CONCATENATE($D$129,C131)</f>
-        <v>wizard.featurePage.featureScreen</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D132" s="2" t="str">
-        <f>CONCATENATE($D$129,C132)</f>
-        <v>wizard.featurePage.keyValueBox</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D134" s="2" t="str">
-        <f>CONCATENATE($C$117,C134)</f>
-        <v>wizard.advertizingPage</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D136" s="2" t="str">
-        <f>CONCATENATE($C$117,C136)</f>
-        <v>wizard.stylePage</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D138" s="2" t="str">
-        <f>CONCATENATE($C$117,C138)</f>
-        <v>wizard.contentPage.</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D139" s="2" t="str">
-        <f>CONCATENATE($D$138,C139)</f>
-        <v>wizard.contentPage.all</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D141" s="2" t="str">
-        <f>CONCATENATE($C$117,C141)</f>
-        <v>wizard.previewPlayerPage.</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D142" s="2" t="str">
-        <f t="shared" ref="D142:D147" si="11">CONCATENATE($D$141,C142)</f>
-        <v>wizard.previewPlayerPage.controls</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="C143" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D143" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>wizard.previewPlayerPage.openClosePreview</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+        <v>wizard.previewPlayerPage.kdpWidth</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>229</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D144" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>wizard.previewPlayerPage.kdpWidth</v>
+        <v>wizard.previewPlayerPage.kdpHeight</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D145" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>wizard.previewPlayerPage.kdpHeight</v>
+        <v>wizard.previewPlayerPage.refreshKdp3</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D146" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>wizard.previewPlayerPage.refreshKdp3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D147" s="2" t="str">
-        <f t="shared" si="11"/>
         <v>wizard.previewPlayerPage.autoPreview</v>
       </c>
     </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="151" spans="1:6">
-      <c r="A151" s="7" t="s">
-        <v>84</v>
+      <c r="A151" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="152" spans="1:6">
-      <c r="A152" s="2" t="s">
-        <v>322</v>
+      <c r="A152" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F152" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D153" s="2" t="str">
+        <f>CONCATENATE($C$152,C153)</f>
+        <v>content.manage.entryTable</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D155" s="2" t="str">
+        <f>CONCATENATE($C$152,C155)</f>
+        <v>content.manage.toolBar.</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F155" s="2" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D154" s="2" t="str">
-        <f>CONCATENATE($C$153,C154)</f>
-        <v>content.manage.entryTable</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D156" s="2" t="str">
-        <f>CONCATENATE($C$153,C156)</f>
-        <v>content.manage.toolBar.</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>95</v>
+        <f>CONCATENATE($D$155,C156)</f>
+        <v>content.manage.toolBar.deleteBtn</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D157" s="2" t="str">
-        <f>CONCATENATE($D$156,C157)</f>
-        <v>content.manage.toolBar.deleteBtn</v>
+        <f t="shared" ref="D157:D161" si="12">CONCATENATE($D$155,C157)</f>
+        <v>content.manage.toolBar.newStreamBtn</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D158" s="2" t="str">
-        <f t="shared" ref="D158:D162" si="12">CONCATENATE($D$156,C158)</f>
-        <v>content.manage.toolBar.newStreamBtn</v>
+        <f t="shared" si="12"/>
+        <v>content.manage.toolBar.download</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D159" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>content.manage.toolBar.download</v>
+        <v>content.manage.toolBar.tagsCombo</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D160" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>content.manage.toolBar.tagsCombo</v>
+        <v>content.manage.toolBar.playlistCombo</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D161" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>content.manage.toolBar.playlistCombo</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D162" s="2" t="str">
-        <f t="shared" si="12"/>
         <v>content.manage.toolBar.moreOption</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D163" s="2" t="str">
+        <f>CONCATENATE($C$152,C163)</f>
+        <v>content.manage.filter.</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D164" s="2" t="str">
-        <f>CONCATENATE($C$153,C164)</f>
-        <v>content.manage.filter.</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>95</v>
+        <f>CONCATENATE($D$163,C164)</f>
+        <v>content.manage.filter.searchBox</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D165" s="2" t="str">
-        <f>CONCATENATE($D$164,C165)</f>
-        <v>content.manage.filter.searchBox</v>
+        <f t="shared" ref="D165:D173" si="13">CONCATENATE($D$163,C165)</f>
+        <v>content.manage.filter.dateCont</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D166" s="2" t="str">
-        <f t="shared" ref="D166:D174" si="13">CONCATENATE($D$164,C166)</f>
-        <v>content.manage.filter.dateCont</v>
+        <f t="shared" si="13"/>
+        <v>content.manage.filter.mediaTypes</v>
       </c>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D167" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.mediaTypes</v>
+        <v>content.manage.filter.conversionStatus</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D168" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.conversionStatus</v>
+        <v>content.manage.filter.durationStatus</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D169" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.durationStatus</v>
+        <v>content.manage.filter.scheduling</v>
       </c>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D170" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.scheduling</v>
+        <v>content.manage.filter.moderationStatus</v>
       </c>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D171" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.moderationStatus</v>
+        <v>content.manage.filter.accessControl</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D172" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.accessControl</v>
+        <v>content.manage.filter.transcodingFlavor</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D173" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>content.manage.filter.transcodingFlavor</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6">
-      <c r="A174" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D174" s="2" t="str">
-        <f t="shared" si="13"/>
         <v>content.manage.filter.categoriesBox</v>
       </c>
     </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
     <row r="176" spans="1:6">
-      <c r="A176" s="5" t="s">
-        <v>131</v>
+      <c r="A176" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
+        <v>110</v>
+      </c>
+      <c r="D176" s="2" t="str">
+        <f>CONCATENATE($C$175,C176)</f>
+        <v>content.moderation.filter.</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D177" s="2" t="str">
-        <f>CONCATENATE($C$176,C177)</f>
-        <v>content.moderation.filter.</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F177" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
+        <f>CONCATENATE($D$163,C177)</f>
+        <v>content.manage.filter.searchBox</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D178" s="2" t="str">
-        <f>CONCATENATE($D$164,C178)</f>
-        <v>content.manage.filter.searchBox</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
+        <f t="shared" ref="D178:D186" si="14">CONCATENATE($D$163,C178)</f>
+        <v>content.manage.filter.dateCont</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D179" s="2" t="str">
-        <f t="shared" ref="D179:D187" si="14">CONCATENATE($D$164,C179)</f>
-        <v>content.manage.filter.dateCont</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
+        <f t="shared" si="14"/>
+        <v>content.manage.filter.mediaTypes</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D180" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.mediaTypes</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
+        <v>content.manage.filter.conversionStatus</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D181" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.conversionStatus</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D182" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.durationStatus</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6">
+        <v>content.manage.filter.scheduling</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D183" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.scheduling</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6">
+        <v>content.manage.filter.moderationStatus</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D184" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.moderationStatus</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6">
+        <v>content.manage.filter.accessControl</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D185" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.accessControl</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6">
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D186" s="2" t="str">
         <f t="shared" si="14"/>
-        <v>content.manage.filter.transcodingFlavor</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6">
-      <c r="A187" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D187" s="2" t="str">
-        <f t="shared" si="14"/>
         <v>content.manage.filter.categoriesBox</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="188" spans="1:4">
+      <c r="A188" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D188" s="2" t="str">
+        <f>CONCATENATE($C$175,C188)</f>
+        <v>content.moderation.entryTable</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D189" s="2" t="str">
-        <f>CONCATENATE($C$176,C189)</f>
-        <v>content.moderation.entryTable</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6">
+        <f>CONCATENATE($C$175,C189)</f>
+        <v>content.moderation.toolBar.</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="2" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="D190" s="2" t="str">
-        <f>CONCATENATE($C$176,C190)</f>
-        <v>content.moderation.toolBar.</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6">
+        <f>CONCATENATE($D$189,C190)</f>
+        <v>content.moderation.toolBar.approveSelected</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D191" s="2" t="str">
-        <f>CONCATENATE($D$190,C191)</f>
-        <v>content.moderation.toolBar.approveSelected</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6">
-      <c r="A192" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D192" s="2" t="str">
-        <f>CONCATENATE($D$190,C192)</f>
+        <f>CONCATENATE($D$189,C191)</f>
         <v>content.moderation.toolBar.rejectSelected</v>
       </c>
     </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="194" spans="1:4">
-      <c r="A194" s="5" t="s">
-        <v>130</v>
+      <c r="A194" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>137</v>
+        <v>107</v>
+      </c>
+      <c r="D194" s="2" t="str">
+        <f>CONCATENATE($C$193,C194)</f>
+        <v>content.playlists.filter</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>CONCATENATE($C$194,C195)</f>
-        <v>content.playlists.filter</v>
+        <f>CONCATENATE($D$194,C195)</f>
+        <v>content.playlists.filterfreeText</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>CONCATENATE($D$195,C196)</f>
-        <v>content.playlists.filterfreeText</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="A197" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D197" s="2" t="str">
-        <f>CONCATENATE($D$195,C197)</f>
+        <f>CONCATENATE($D$194,C196)</f>
         <v>content.playlists.filterdateCont</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D198" s="2" t="str">
+        <f t="shared" ref="D198:D204" si="15">CONCATENATE($C$193,C198)</f>
+        <v>content.playlists.entryTableContainer</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f t="shared" ref="D199:D205" si="15">CONCATENATE($C$194,C199)</f>
-        <v>content.playlists.entryTableContainer</v>
+        <f t="shared" si="15"/>
+        <v>content.playlists.toolBar.</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D200" s="2" t="str">
+        <f>CONCATENATE($D$199,C200)</f>
+        <v>content.playlists.toolBar.deleteBtn</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D202" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>content.playlists.toolBar.</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4">
-      <c r="A201" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D201" s="2" t="str">
-        <f>CONCATENATE($D$200,C201)</f>
-        <v>content.playlists.toolBar.deleteBtn</v>
+        <v>content.playlists.actionsBox</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D203" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>content.playlists.actionsBox</v>
+        <v>content.playlists.addManualPlaylistBtn</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D204" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>content.playlists.addManualPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
-      <c r="A205" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D205" s="2" t="str">
-        <f t="shared" si="15"/>
         <v>content.playlists.addRuleBasedPlaylistBtn</v>
       </c>
     </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="5" t="s">
-        <v>146</v>
+      <c r="A207" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="D207" s="2" t="str">
+        <f>CONCATENATE($C$206,C207)</f>
+        <v>content.syndication.feedsTable</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D208" s="2" t="str">
-        <f>CONCATENATE($C$207,C208)</f>
-        <v>content.syndication.feedsTable</v>
+        <f>CONCATENATE($C$206,C208)</f>
+        <v>content.syndication.deleteExSynBtn</v>
       </c>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D209" s="2" t="str">
-        <f>CONCATENATE($C$207,C209)</f>
-        <v>content.syndication.deleteExSynBtn</v>
+        <f t="shared" ref="D209:D210" si="16">CONCATENATE($C$206,C209)</f>
+        <v>content.syndication.actionsBox</v>
       </c>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="D210" s="2" t="str">
-        <f t="shared" ref="D210:D211" si="16">CONCATENATE($C$207,C210)</f>
-        <v>content.syndication.actionsBox</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7">
-      <c r="A211" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D211" s="2" t="str">
         <f t="shared" si="16"/>
         <v>content.syndication.addBtn</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
-      <c r="A213" s="8" t="s">
+    <row r="212" spans="1:7">
+      <c r="A212" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="C212" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E213" s="2" t="s">
+      <c r="E212" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F213" s="2" t="s">
+      <c r="F212" s="2" t="s">
         <v>173</v>
       </c>
     </row>
+    <row r="214" spans="1:7">
+      <c r="A214" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="5" t="s">
-        <v>154</v>
+      <c r="A215" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
+      </c>
+      <c r="D215" s="2" t="str">
+        <f>CONCATENATE($C$214,C215)</f>
+        <v>content.upload.kcwBox</v>
       </c>
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D216" s="2" t="str">
-        <f>CONCATENATE($C$215,C216)</f>
-        <v>content.upload.kcwBox</v>
+        <f t="shared" ref="D216:D217" si="17">CONCATENATE($C$214,C216)</f>
+        <v>content.upload.profilesCb</v>
       </c>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D217" s="2" t="str">
-        <f t="shared" ref="D217:D218" si="17">CONCATENATE($C$215,C217)</f>
-        <v>content.upload.profilesCb</v>
+        <f t="shared" si="17"/>
+        <v>content.upload.kcwBtn</v>
       </c>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D218" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v>content.upload.kcwBtn</v>
+        <f t="shared" ref="D218:D219" si="18">CONCATENATE($C$214,C218)</f>
+        <v>content.upload.bulkUploadBox</v>
       </c>
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D219" s="2" t="str">
-        <f t="shared" ref="D219:D220" si="18">CONCATENATE($C$215,C219)</f>
-        <v>content.upload.bulkUploadBox</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7">
-      <c r="A220" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D220" s="2" t="str">
         <f t="shared" si="18"/>
         <v>content.upload.submitBtn</v>
       </c>
     </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G221" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="222" spans="1:7">
-      <c r="A222" s="8" t="s">
-        <v>160</v>
+      <c r="A222" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E222" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F222" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G222" s="2" t="s">
-        <v>76</v>
+        <v>176</v>
+      </c>
+      <c r="D222" s="2" t="str">
+        <f>CONCATENATE($C$221,C222)</f>
+        <v>entryDrilldown.entryMetaData.</v>
       </c>
     </row>
     <row r="223" spans="1:7">
       <c r="A223" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D223" s="2" t="str">
-        <f>CONCATENATE($C$222,C223)</f>
-        <v>entryDrilldown.entryMetaData.</v>
+        <f>CONCATENATE($D$222,C223)</f>
+        <v>entryDrilldown.entryMetaData.name_input</v>
       </c>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D224" s="2" t="str">
-        <f>CONCATENATE($D$223,C224)</f>
-        <v>entryDrilldown.entryMetaData.name_input</v>
+        <f t="shared" ref="D224:D227" si="19">CONCATENATE($D$222,C224)</f>
+        <v>entryDrilldown.entryMetaData.descriptionTi</v>
       </c>
     </row>
     <row r="225" spans="1:7">
       <c r="A225" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D225" s="2" t="str">
-        <f t="shared" ref="D225:D228" si="19">CONCATENATE($D$223,C225)</f>
-        <v>entryDrilldown.entryMetaData.descriptionTi</v>
+        <f t="shared" si="19"/>
+        <v>entryDrilldown.entryMetaData.tagsTi</v>
       </c>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D226" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>entryDrilldown.entryMetaData.tagsTi</v>
+        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
       </c>
     </row>
     <row r="227" spans="1:7">
       <c r="A227" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>185</v>
+        <v>6</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D227" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7">
-      <c r="A228" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D228" s="2" t="str">
-        <f t="shared" si="19"/>
         <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
       </c>
     </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D229" s="2" t="str">
+        <f>CONCATENATE($C$221,C229)</f>
+        <v>entryDrilldown.entrySch.</v>
+      </c>
+      <c r="E229" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F229" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G229" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="2" t="s">
+      <c r="B230" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D230" s="2" t="str">
+        <f>CONCATENATE($D$229,C230)</f>
+        <v>entryDrilldown.entrySch.anyTimeRBtn</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
+      <c r="B231" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D231" s="2" t="str">
+        <f t="shared" ref="D231:D237" si="20">CONCATENATE($D$229,C231)</f>
+        <v>entryDrilldown.entrySch.spcificRangeRBtn</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="B232" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D232" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.sepcificStartDate</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
+      <c r="B233" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D233" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.sepcificStartHour</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="B234" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D234" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.specificEndCBBtn</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
+      <c r="B235" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D235" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.specificEndDate</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
+      <c r="B236" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D236" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.specificEndHour</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
+      <c r="B237" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D237" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>entryDrilldown.entrySch.clearDatesBtn</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B230" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C230" s="2" t="s">
+      <c r="B239" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C239" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D230" s="2" t="str">
-        <f>CONCATENATE($C$222,C230)</f>
+      <c r="D239" s="2" t="str">
+        <f>CONCATENATE($C$221,C239)</f>
         <v>entryDrilldown.entryAcp.</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
-      <c r="A231" s="2" t="s">
+    <row r="240" spans="1:7">
+      <c r="A240" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B240" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="C240" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D231" s="2" t="str">
-        <f>CONCATENATE($D$230,C231)</f>
+      <c r="D240" s="2" t="str">
+        <f>CONCATENATE($D$239,C240)</f>
         <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
-      <c r="A232" s="2" t="s">
+    <row r="241" spans="1:7">
+      <c r="A241" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B241" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C241" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D232" s="2" t="str">
-        <f>CONCATENATE($D$230,C232)</f>
+      <c r="D241" s="2" t="str">
+        <f>CONCATENATE($D$239,C241)</f>
         <v>entryDrilldown.entryAcp.addBtn</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
-      <c r="A234" s="2" t="s">
+    <row r="243" spans="1:7">
+      <c r="A243" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B234" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C234" s="2" t="s">
+      <c r="B243" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D234" s="2" t="str">
-        <f>CONCATENATE($C$222,C234)</f>
+      <c r="D243" s="2" t="str">
+        <f>CONCATENATE($C$221,C243)</f>
         <v>entryDrilldown.customData</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
-      <c r="A236" s="2" t="s">
+    <row r="245" spans="1:7">
+      <c r="A245" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B236" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C236" s="2" t="s">
+      <c r="B245" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D236" s="2" t="str">
-        <f>CONCATENATE($C$222,C236)</f>
+      <c r="D245" s="2" t="str">
+        <f>CONCATENATE($C$221,C245)</f>
         <v>entryDrilldown.entryAsstes</v>
       </c>
-      <c r="E236" s="2" t="s">
+      <c r="E245" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F236" s="2" t="s">
+      <c r="F245" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G236" s="2" t="s">
+      <c r="G245" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
-      <c r="A238" s="8" t="s">
+    <row r="247" spans="1:7">
+      <c r="A247" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="C247" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E238" s="2" t="s">
+      <c r="E247" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F238" s="2" t="s">
+      <c r="F247" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="8" t="s">
+    <row r="248" spans="1:7">
+      <c r="A248" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C239" s="2" t="s">
+      <c r="C248" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E239" s="2" t="s">
+      <c r="E248" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F239" s="2" t="s">
+      <c r="F248" s="2" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
admin drilldown windows mapping
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54029 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="373">
   <si>
     <t>Dashboard</t>
   </si>
@@ -1093,6 +1093,48 @@
   </si>
   <si>
     <t>only handles the things that are otherwise bound</t>
+  </si>
+  <si>
+    <t>user drilldown</t>
+  </si>
+  <si>
+    <t>userDrilldown.</t>
+  </si>
+  <si>
+    <t>emailTi</t>
+  </si>
+  <si>
+    <t>firstNameTi</t>
+  </si>
+  <si>
+    <t>lastNameTi</t>
+  </si>
+  <si>
+    <t>roleCb</t>
+  </si>
+  <si>
+    <t>addRoleBtn</t>
+  </si>
+  <si>
+    <t>role drilldown</t>
+  </si>
+  <si>
+    <t>roleDrilldown.</t>
+  </si>
+  <si>
+    <t>nameTi</t>
+  </si>
+  <si>
+    <t>myForm</t>
+  </si>
+  <si>
+    <t>dynamic form container</t>
+  </si>
+  <si>
+    <t>role description</t>
+  </si>
+  <si>
+    <t>role name</t>
   </si>
 </sst>
 </file>
@@ -1478,11 +1520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G248"/>
+  <dimension ref="A1:G262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D230" sqref="D230:D237"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2741,1713 +2783,1881 @@
         <v>76</v>
       </c>
     </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+    </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>65</v>
+      <c r="A106" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="107" spans="1:7">
-      <c r="A107" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>32</v>
+      <c r="A107" s="4"/>
+      <c r="B107" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>32</v>
+        <v>361</v>
       </c>
       <c r="D107" s="2" t="str">
-        <f>CONCATENATE($C$100,C107)</f>
-        <v>admin.users.table</v>
+        <f>CONCATENATE($C$106,C107)</f>
+        <v>userDrilldown.emailTi</v>
       </c>
     </row>
     <row r="108" spans="1:7">
-      <c r="A108" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>22</v>
+      <c r="A108" s="4"/>
+      <c r="B108" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>61</v>
+        <v>362</v>
       </c>
       <c r="D108" s="2" t="str">
-        <f>CONCATENATE($C$100,C108)</f>
-        <v>admin.users.addBtn</v>
+        <f t="shared" ref="D108:D112" si="9">CONCATENATE($C$106,C108)</f>
+        <v>userDrilldown.firstNameTi</v>
       </c>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>6</v>
+      <c r="A109" s="4"/>
+      <c r="B109" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>63</v>
+        <v>363</v>
       </c>
       <c r="D109" s="2" t="str">
-        <f>CONCATENATE($C$100,C109)</f>
-        <v>admin.users.actionButtonsContainer</v>
+        <f t="shared" si="9"/>
+        <v>userDrilldown.lastNameTi</v>
       </c>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>32</v>
+        <v>364</v>
       </c>
       <c r="D110" s="2" t="str">
-        <f>CONCATENATE($C$100,C110)</f>
-        <v>admin.users.table</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="7" t="s">
-        <v>67</v>
+        <f t="shared" si="9"/>
+        <v>userDrilldown.roleCb</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D111" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>userDrilldown.addRoleBtn</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D112" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>userDrilldown.saveBtn</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="2" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="D115" s="2" t="str">
         <f>CONCATENATE($C$114,C115)</f>
-        <v>studio.playerList.templatesHolder</v>
+        <v>admin.roles.table</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
+      </c>
+      <c r="D116" s="2" t="str">
+        <f t="shared" ref="D116:D118" si="10">CONCATENATE($C$114,C116)</f>
+        <v>admin.roles.addBtn</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>admin.roles.actionButtonsContainer</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>admin.roles.table</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D121" s="2" t="str">
+        <f>CONCATENATE($C$106,C121)</f>
+        <v>userDrilldown.nameTi</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D122" s="2" t="str">
+        <f t="shared" ref="D122:D124" si="11">CONCATENATE($C$106,C122)</f>
+        <v>userDrilldown.descriptionTi</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>userDrilldown.saveBtn</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D124" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>userDrilldown.myForm</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D129" s="2" t="str">
+        <f>CONCATENATE($C$128,C129)</f>
+        <v>studio.playerList.templatesHolder</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="2" t="str">
-        <f>CONCATENATE($C$116,C117)</f>
+      <c r="D131" s="2" t="str">
+        <f>CONCATENATE($C$130,C131)</f>
         <v>wizard.wizardSaveBtn</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="1" t="s">
+    <row r="132" spans="1:7">
+      <c r="A132" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B118" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="1" t="s">
+      <c r="B132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D118" s="1" t="str">
-        <f t="shared" ref="D118" si="9">CONCATENATE($C$116,C118)</f>
+      <c r="D132" s="1" t="str">
+        <f t="shared" ref="D132" si="12">CONCATENATE($C$130,C132)</f>
         <v>wizard.templatePage.</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="1" t="s">
+    <row r="133" spans="1:7">
+      <c r="A133" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="1" t="s">
+      <c r="B133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D119" s="1" t="str">
-        <f t="shared" ref="D119:D126" si="10">CONCATENATE($D$118,C119)</f>
+      <c r="D133" s="1" t="str">
+        <f t="shared" ref="D133:D140" si="13">CONCATENATE($D$132,C133)</f>
         <v>wizard.templatePage.all</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="1" t="s">
+    <row r="134" spans="1:7">
+      <c r="A134" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C134" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D120" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D134" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.playerName</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
-      <c r="A121" s="1" t="s">
+    <row r="135" spans="1:7">
+      <c r="A135" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C135" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D121" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D135" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.keepOriginalRatio</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
-      <c r="A122" s="1" t="s">
+    <row r="136" spans="1:7">
+      <c r="A136" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D122" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D136" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.streachMediaToFitPlayer</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
-      <c r="A123" s="1" t="s">
+    <row r="137" spans="1:7">
+      <c r="A137" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B137" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D123" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D137" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.templateAutoPlay</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="1" t="s">
+    <row r="138" spans="1:7">
+      <c r="A138" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B138" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D124" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D138" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.templateAutoMute</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="1" t="s">
+    <row r="139" spans="1:7">
+      <c r="A139" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C139" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D125" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D139" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.playlistAutoContinue</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
-      <c r="A126" s="1" t="s">
+    <row r="140" spans="1:7">
+      <c r="A140" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D126" s="1" t="str">
-        <f t="shared" si="10"/>
+      <c r="D140" s="1" t="str">
+        <f t="shared" si="13"/>
         <v>wizard.templatePage.playlistImagesInterval</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
-      <c r="A128" s="2" t="s">
+    <row r="142" spans="1:7">
+      <c r="A142" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128" s="2" t="s">
+      <c r="B142" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D128" s="2" t="str">
-        <f>CONCATENATE($C$116,C128)</f>
+      <c r="D142" s="2" t="str">
+        <f>CONCATENATE($C$130,C142)</f>
         <v>wizard.featurePage.</v>
       </c>
-      <c r="E128" s="2" t="s">
+      <c r="E142" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F142" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="3" t="s">
+    <row r="143" spans="1:7">
+      <c r="A143" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D129" s="2" t="str">
-        <f>CONCATENATE($D$128,C129)</f>
+      <c r="D143" s="2" t="str">
+        <f>CONCATENATE($D$142,C143)</f>
         <v>wizard.featurePage.accordi</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="3" t="s">
+    <row r="144" spans="1:7">
+      <c r="A144" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130" s="2" t="s">
+      <c r="B144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D130" s="2" t="str">
-        <f>CONCATENATE($D$128,C130)</f>
+      <c r="D144" s="2" t="str">
+        <f>CONCATENATE($D$142,C144)</f>
         <v>wizard.featurePage.featureScreen</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="3" t="s">
+    <row r="145" spans="1:4">
+      <c r="A145" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B131" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131" s="2" t="s">
+      <c r="B145" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D131" s="2" t="str">
-        <f>CONCATENATE($D$128,C131)</f>
+      <c r="D145" s="2" t="str">
+        <f>CONCATENATE($D$142,C145)</f>
         <v>wizard.featurePage.keyValueBox</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="2" t="s">
+    <row r="147" spans="1:4">
+      <c r="A147" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C133" s="2" t="s">
+      <c r="B147" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D133" s="2" t="str">
-        <f>CONCATENATE($C$116,C133)</f>
+      <c r="D147" s="2" t="str">
+        <f>CONCATENATE($C$130,C147)</f>
         <v>wizard.advertizingPage</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="2" t="s">
+    <row r="149" spans="1:4">
+      <c r="A149" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C135" s="2" t="s">
+      <c r="B149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D135" s="2" t="str">
-        <f>CONCATENATE($C$116,C135)</f>
+      <c r="D149" s="2" t="str">
+        <f>CONCATENATE($C$130,C149)</f>
         <v>wizard.stylePage</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="2" t="s">
+    <row r="151" spans="1:4">
+      <c r="A151" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137" s="2" t="s">
+      <c r="B151" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D137" s="2" t="str">
-        <f>CONCATENATE($C$116,C137)</f>
+      <c r="D151" s="2" t="str">
+        <f>CONCATENATE($C$130,C151)</f>
         <v>wizard.contentPage.</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="2" t="s">
+    <row r="152" spans="1:4">
+      <c r="A152" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138" s="2" t="s">
+      <c r="B152" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D138" s="2" t="str">
-        <f>CONCATENATE($D$137,C138)</f>
+      <c r="D152" s="2" t="str">
+        <f>CONCATENATE($D$151,C152)</f>
         <v>wizard.contentPage.all</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
-      <c r="A140" s="2" t="s">
+    <row r="154" spans="1:4">
+      <c r="A154" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C140" s="2" t="s">
+      <c r="B154" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D140" s="2" t="str">
-        <f>CONCATENATE($C$116,C140)</f>
+      <c r="D154" s="2" t="str">
+        <f>CONCATENATE($C$130,C154)</f>
         <v>wizard.previewPlayerPage.</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="2" t="s">
+    <row r="155" spans="1:4">
+      <c r="A155" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141" s="2" t="s">
+      <c r="B155" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D141" s="2" t="str">
-        <f t="shared" ref="D141:D146" si="11">CONCATENATE($D$140,C141)</f>
+      <c r="D155" s="2" t="str">
+        <f t="shared" ref="D155:D160" si="14">CONCATENATE($D$154,C155)</f>
         <v>wizard.previewPlayerPage.controls</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="2" t="s">
+    <row r="156" spans="1:4">
+      <c r="A156" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D142" s="2" t="str">
-        <f t="shared" si="11"/>
+      <c r="D156" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>wizard.previewPlayerPage.openClosePreview</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="2" t="s">
+    <row r="157" spans="1:4">
+      <c r="A157" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D143" s="2" t="str">
-        <f t="shared" si="11"/>
+      <c r="D157" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>wizard.previewPlayerPage.kdpWidth</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="2" t="s">
+    <row r="158" spans="1:4">
+      <c r="A158" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D144" s="2" t="str">
-        <f t="shared" si="11"/>
+      <c r="D158" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>wizard.previewPlayerPage.kdpHeight</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
-      <c r="A145" s="2" t="s">
+    <row r="159" spans="1:4">
+      <c r="A159" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D145" s="2" t="str">
-        <f t="shared" si="11"/>
+      <c r="D159" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>wizard.previewPlayerPage.refreshKdp3</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
-      <c r="A146" s="2" t="s">
+    <row r="160" spans="1:4">
+      <c r="A160" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D146" s="2" t="str">
-        <f t="shared" si="11"/>
+      <c r="D160" s="2" t="str">
+        <f t="shared" si="14"/>
         <v>wizard.previewPlayerPage.autoPreview</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
-      <c r="A150" s="7" t="s">
+    <row r="164" spans="1:6">
+      <c r="A164" s="7" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D153" s="2" t="str">
-        <f>CONCATENATE($C$152,C153)</f>
-        <v>content.manage.entryTable</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D155" s="2" t="str">
-        <f>CONCATENATE($C$152,C155)</f>
-        <v>content.manage.toolBar.</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D156" s="2" t="str">
-        <f>CONCATENATE($D$155,C156)</f>
-        <v>content.manage.toolBar.deleteBtn</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D157" s="2" t="str">
-        <f t="shared" ref="D157:D161" si="12">CONCATENATE($D$155,C157)</f>
-        <v>content.manage.toolBar.newStreamBtn</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="A158" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D158" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>content.manage.toolBar.download</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6">
-      <c r="A159" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D159" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>content.manage.toolBar.tagsCombo</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6">
-      <c r="A160" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D160" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>content.manage.toolBar.playlistCombo</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D161" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>content.manage.toolBar.moreOption</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D163" s="2" t="str">
-        <f>CONCATENATE($C$152,C163)</f>
-        <v>content.manage.filter.</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D164" s="2" t="str">
-        <f>CONCATENATE($D$163,C164)</f>
-        <v>content.manage.filter.searchBox</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>6</v>
+        <v>322</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D165" s="2" t="str">
-        <f t="shared" ref="D165:D173" si="13">CONCATENATE($D$163,C165)</f>
-        <v>content.manage.filter.dateCont</v>
+        <v>323</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="166" spans="1:6">
-      <c r="A166" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>6</v>
+      <c r="A166" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D166" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.mediaTypes</v>
+        <v>86</v>
       </c>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" s="2" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D167" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.conversionStatus</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D168" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.durationStatus</v>
+        <f>CONCATENATE($C$166,C167)</f>
+        <v>content.manage.entryTable</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" s="2" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="D169" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.scheduling</v>
+        <f>CONCATENATE($C$166,C169)</f>
+        <v>content.manage.toolBar.</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="2" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="D170" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.moderationStatus</v>
+        <f>CONCATENATE($D$169,C170)</f>
+        <v>content.manage.toolBar.deleteBtn</v>
       </c>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="D171" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.accessControl</v>
+        <f t="shared" ref="D171:D175" si="15">CONCATENATE($D$169,C171)</f>
+        <v>content.manage.toolBar.newStreamBtn</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="2" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="D172" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>content.manage.filter.transcodingFlavor</v>
+        <f t="shared" si="15"/>
+        <v>content.manage.toolBar.download</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D173" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.manage.toolBar.tagsCombo</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D174" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.manage.toolBar.playlistCombo</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D175" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>content.manage.toolBar.moreOption</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D177" s="2" t="str">
+        <f>CONCATENATE($C$166,C177)</f>
+        <v>content.manage.filter.</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D178" s="2" t="str">
+        <f>CONCATENATE($D$177,C178)</f>
+        <v>content.manage.filter.searchBox</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D179" s="2" t="str">
+        <f t="shared" ref="D179:D187" si="16">CONCATENATE($D$177,C179)</f>
+        <v>content.manage.filter.dateCont</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D180" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.mediaTypes</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D181" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.conversionStatus</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D182" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.durationStatus</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D183" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.scheduling</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D184" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.moderationStatus</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D185" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.accessControl</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D186" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>content.manage.filter.transcodingFlavor</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B173" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173" s="2" t="s">
+      <c r="B187" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D173" s="2" t="str">
-        <f t="shared" si="13"/>
+      <c r="D187" s="2" t="str">
+        <f t="shared" si="16"/>
         <v>content.manage.filter.categoriesBox</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
-      <c r="A175" s="5" t="s">
+    <row r="189" spans="1:6">
+      <c r="A189" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C189" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
-      <c r="A176" s="2" t="s">
+    <row r="190" spans="1:6">
+      <c r="A190" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C190" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D176" s="2" t="str">
-        <f>CONCATENATE($C$175,C176)</f>
+      <c r="D190" s="2" t="str">
+        <f>CONCATENATE($C$189,C190)</f>
         <v>content.moderation.filter.</v>
       </c>
-      <c r="E176" s="2" t="s">
+      <c r="E190" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="F190" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="2" t="s">
+    <row r="191" spans="1:6">
+      <c r="A191" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B177" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C177" s="2" t="s">
+      <c r="B191" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D177" s="2" t="str">
-        <f>CONCATENATE($D$163,C177)</f>
+      <c r="D191" s="2" t="str">
+        <f>CONCATENATE($D$177,C191)</f>
         <v>content.manage.filter.searchBox</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="2" t="s">
+    <row r="192" spans="1:6">
+      <c r="A192" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C178" s="2" t="s">
+      <c r="B192" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D178" s="2" t="str">
-        <f t="shared" ref="D178:D186" si="14">CONCATENATE($D$163,C178)</f>
+      <c r="D192" s="2" t="str">
+        <f t="shared" ref="D192:D200" si="17">CONCATENATE($D$177,C192)</f>
         <v>content.manage.filter.dateCont</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="2" t="s">
+    <row r="193" spans="1:4">
+      <c r="A193" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B179" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C179" s="2" t="s">
+      <c r="B193" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D179" s="2" t="str">
-        <f t="shared" si="14"/>
+      <c r="D193" s="2" t="str">
+        <f t="shared" si="17"/>
         <v>content.manage.filter.mediaTypes</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4">
-      <c r="A180" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D180" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.conversionStatus</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
-      <c r="A181" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D181" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.durationStatus</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
-      <c r="A182" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D182" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.scheduling</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="A183" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D183" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.moderationStatus</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="A184" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D184" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.accessControl</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
-      <c r="A185" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D185" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.transcodingFlavor</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
-      <c r="A186" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D186" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>content.manage.filter.categoriesBox</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D188" s="2" t="str">
-        <f>CONCATENATE($C$175,C188)</f>
-        <v>content.moderation.entryTable</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D189" s="2" t="str">
-        <f>CONCATENATE($C$175,C189)</f>
-        <v>content.moderation.toolBar.</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
-      <c r="A190" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D190" s="2" t="str">
-        <f>CONCATENATE($D$189,C190)</f>
-        <v>content.moderation.toolBar.approveSelected</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D191" s="2" t="str">
-        <f>CONCATENATE($D$189,C191)</f>
-        <v>content.moderation.toolBar.rejectSelected</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
-      <c r="A193" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D194" s="2" t="str">
-        <f>CONCATENATE($C$193,C194)</f>
-        <v>content.playlists.filter</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.conversionStatus</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D195" s="2" t="str">
-        <f>CONCATENATE($D$194,C195)</f>
-        <v>content.playlists.filterfreeText</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.durationStatus</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D196" s="2" t="str">
-        <f>CONCATENATE($D$194,C196)</f>
-        <v>content.playlists.filterdateCont</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.scheduling</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D197" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.moderationStatus</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="2" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D198" s="2" t="str">
-        <f t="shared" ref="D198:D204" si="15">CONCATENATE($C$193,C198)</f>
-        <v>content.playlists.entryTableContainer</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.accessControl</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="2" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="D199" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>content.playlists.toolBar.</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.transcodingFlavor</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="2" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="D200" s="2" t="str">
-        <f>CONCATENATE($D$199,C200)</f>
-        <v>content.playlists.toolBar.deleteBtn</v>
+        <f t="shared" si="17"/>
+        <v>content.manage.filter.categoriesBox</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="2" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="D202" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>content.playlists.actionsBox</v>
+        <f>CONCATENATE($C$189,C202)</f>
+        <v>content.moderation.entryTable</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="2" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="D203" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>content.playlists.addManualPlaylistBtn</v>
+        <f>CONCATENATE($C$189,C203)</f>
+        <v>content.moderation.toolBar.</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D204" s="2" t="str">
-        <f t="shared" si="15"/>
-        <v>content.playlists.addRuleBasedPlaylistBtn</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4">
-      <c r="A206" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>147</v>
+        <f>CONCATENATE($D$203,C204)</f>
+        <v>content.moderation.toolBar.approveSelected</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D205" s="2" t="str">
+        <f>CONCATENATE($D$203,C205)</f>
+        <v>content.moderation.toolBar.rejectSelected</v>
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>32</v>
+      <c r="A207" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D207" s="2" t="str">
-        <f>CONCATENATE($C$206,C207)</f>
-        <v>content.syndication.feedsTable</v>
+        <v>137</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="2" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="B208" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D208" s="2" t="str">
+        <f>CONCATENATE($C$207,C208)</f>
+        <v>content.playlists.filter</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D209" s="2" t="str">
+        <f>CONCATENATE($D$208,C209)</f>
+        <v>content.playlists.filterfreeText</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D210" s="2" t="str">
+        <f>CONCATENATE($D$208,C210)</f>
+        <v>content.playlists.filterdateCont</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D212" s="2" t="str">
+        <f t="shared" ref="D212:D218" si="18">CONCATENATE($C$207,C212)</f>
+        <v>content.playlists.entryTableContainer</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D213" s="2" t="str">
+        <f t="shared" si="18"/>
+        <v>content.playlists.toolBar.</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C208" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D208" s="2" t="str">
-        <f>CONCATENATE($C$206,C208)</f>
-        <v>content.syndication.deleteExSynBtn</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="A209" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C209" s="2" t="s">
+      <c r="C214" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D214" s="2" t="str">
+        <f>CONCATENATE($D$213,C214)</f>
+        <v>content.playlists.toolBar.deleteBtn</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D209" s="2" t="str">
-        <f t="shared" ref="D209:D210" si="16">CONCATENATE($C$206,C209)</f>
-        <v>content.syndication.actionsBox</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7">
-      <c r="A210" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D210" s="2" t="str">
-        <f t="shared" si="16"/>
-        <v>content.syndication.addBtn</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7">
-      <c r="A212" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F212" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7">
-      <c r="A214" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7">
-      <c r="A215" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D215" s="2" t="str">
-        <f>CONCATENATE($C$214,C215)</f>
-        <v>content.upload.kcwBox</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="A216" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="D216" s="2" t="str">
-        <f t="shared" ref="D216:D217" si="17">CONCATENATE($C$214,C216)</f>
-        <v>content.upload.profilesCb</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7">
+        <f t="shared" si="18"/>
+        <v>content.playlists.actionsBox</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
       <c r="A217" s="2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C217" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D217" s="2" t="str">
+        <f t="shared" si="18"/>
+        <v>content.playlists.addManualPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D218" s="2" t="str">
+        <f t="shared" si="18"/>
+        <v>content.playlists.addRuleBasedPlaylistBtn</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D221" s="2" t="str">
+        <f>CONCATENATE($C$220,C221)</f>
+        <v>content.syndication.feedsTable</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D222" s="2" t="str">
+        <f>CONCATENATE($C$220,C222)</f>
+        <v>content.syndication.deleteExSynBtn</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D223" s="2" t="str">
+        <f t="shared" ref="D223:D224" si="19">CONCATENATE($C$220,C223)</f>
+        <v>content.syndication.actionsBox</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D224" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>content.syndication.addBtn</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7">
+      <c r="A226" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F226" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7">
+      <c r="A228" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D229" s="2" t="str">
+        <f>CONCATENATE($C$228,C229)</f>
+        <v>content.upload.kcwBox</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D230" s="2" t="str">
+        <f t="shared" ref="D230:D231" si="20">CONCATENATE($C$228,C230)</f>
+        <v>content.upload.profilesCb</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
+      <c r="A231" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C231" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D217" s="2" t="str">
-        <f t="shared" si="17"/>
+      <c r="D231" s="2" t="str">
+        <f t="shared" si="20"/>
         <v>content.upload.kcwBtn</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
-      <c r="A218" s="2" t="s">
+    <row r="232" spans="1:7">
+      <c r="A232" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C218" s="2" t="s">
+      <c r="C232" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D218" s="2" t="str">
-        <f t="shared" ref="D218:D219" si="18">CONCATENATE($C$214,C218)</f>
+      <c r="D232" s="2" t="str">
+        <f t="shared" ref="D232:D233" si="21">CONCATENATE($C$228,C232)</f>
         <v>content.upload.bulkUploadBox</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
-      <c r="A219" s="2" t="s">
+    <row r="233" spans="1:7">
+      <c r="A233" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B233" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C233" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D219" s="2" t="str">
-        <f t="shared" si="18"/>
+      <c r="D233" s="2" t="str">
+        <f t="shared" si="21"/>
         <v>content.upload.submitBtn</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
-      <c r="A221" s="8" t="s">
+    <row r="235" spans="1:7">
+      <c r="A235" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="C235" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E221" s="2" t="s">
+      <c r="E235" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F221" s="2" t="s">
+      <c r="F235" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G221" s="2" t="s">
+      <c r="G235" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
-      <c r="A222" s="2" t="s">
+    <row r="236" spans="1:7">
+      <c r="A236" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C222" s="2" t="s">
+      <c r="B236" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D222" s="2" t="str">
-        <f>CONCATENATE($C$221,C222)</f>
+      <c r="D236" s="2" t="str">
+        <f>CONCATENATE($C$235,C236)</f>
         <v>entryDrilldown.entryMetaData.</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="2" t="s">
+    <row r="237" spans="1:7">
+      <c r="A237" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="B237" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="C237" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D223" s="2" t="str">
-        <f>CONCATENATE($D$222,C223)</f>
+      <c r="D237" s="2" t="str">
+        <f>CONCATENATE($D$236,C237)</f>
         <v>entryDrilldown.entryMetaData.name_input</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
-      <c r="A224" s="2" t="s">
+    <row r="238" spans="1:7">
+      <c r="A238" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B238" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C238" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D224" s="2" t="str">
-        <f t="shared" ref="D224:D227" si="19">CONCATENATE($D$222,C224)</f>
+      <c r="D238" s="2" t="str">
+        <f>CONCATENATE($D$236,C238)</f>
         <v>entryDrilldown.entryMetaData.descriptionTi</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7">
-      <c r="A225" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D225" s="2" t="str">
-        <f t="shared" si="19"/>
-        <v>entryDrilldown.entryMetaData.tagsTi</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7">
-      <c r="A226" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D226" s="2" t="str">
-        <f t="shared" si="19"/>
-        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7">
-      <c r="A227" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D227" s="2" t="str">
-        <f t="shared" si="19"/>
-        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7">
-      <c r="A229" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="D229" s="2" t="str">
-        <f>CONCATENATE($C$221,C229)</f>
-        <v>entryDrilldown.entrySch.</v>
-      </c>
-      <c r="E229" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F229" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G229" s="4" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="230" spans="1:7">
-      <c r="B230" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="D230" s="2" t="str">
-        <f>CONCATENATE($D$229,C230)</f>
-        <v>entryDrilldown.entrySch.anyTimeRBtn</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7">
-      <c r="B231" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="D231" s="2" t="str">
-        <f t="shared" ref="D231:D237" si="20">CONCATENATE($D$229,C231)</f>
-        <v>entryDrilldown.entrySch.spcificRangeRBtn</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7">
-      <c r="B232" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="D232" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.sepcificStartDate</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7">
-      <c r="B233" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="D233" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.sepcificStartHour</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7">
-      <c r="B234" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D234" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.specificEndCBBtn</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7">
-      <c r="B235" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D235" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.specificEndDate</v>
-      </c>
-    </row>
-    <row r="236" spans="1:7">
-      <c r="B236" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D236" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.specificEndHour</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7">
-      <c r="B237" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D237" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>entryDrilldown.entrySch.clearDatesBtn</v>
       </c>
     </row>
     <row r="239" spans="1:7">
       <c r="A239" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D239" s="2" t="str">
-        <f>CONCATENATE($C$221,C239)</f>
-        <v>entryDrilldown.entryAcp.</v>
+        <f>CONCATENATE($D$236,C239)</f>
+        <v>entryDrilldown.entryMetaData.tagsTi</v>
       </c>
     </row>
     <row r="240" spans="1:7">
       <c r="A240" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D240" s="2" t="str">
-        <f>CONCATENATE($D$239,C240)</f>
-        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+        <f>CONCATENATE($D$236,C240)</f>
+        <v>entryDrilldown.entryMetaData.categoriesTextInput</v>
       </c>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D241" s="2" t="str">
+        <f>CONCATENATE($D$236,C241)</f>
+        <v>entryDrilldown.entryMetaData.thumbnailOptionBox</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
+      <c r="A243" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D243" s="2" t="str">
+        <f>CONCATENATE($C$235,C243)</f>
+        <v>entryDrilldown.entrySch.</v>
+      </c>
+      <c r="E243" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F243" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G243" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7">
+      <c r="B244" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D244" s="2" t="str">
+        <f>CONCATENATE($D$243,C244)</f>
+        <v>entryDrilldown.entrySch.anyTimeRBtn</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="B245" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D245" s="2" t="str">
+        <f t="shared" ref="D245:D251" si="22">CONCATENATE($D$243,C245)</f>
+        <v>entryDrilldown.entrySch.spcificRangeRBtn</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="B246" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D246" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.sepcificStartDate</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="B247" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D247" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.sepcificStartHour</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7">
+      <c r="B248" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D248" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.specificEndCBBtn</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="B249" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D249" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.specificEndDate</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7">
+      <c r="B250" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D250" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.specificEndHour</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="B251" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D251" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>entryDrilldown.entrySch.clearDatesBtn</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D253" s="2" t="str">
+        <f>CONCATENATE($C$235,C253)</f>
+        <v>entryDrilldown.entryAcp.</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D254" s="2" t="str">
+        <f>CONCATENATE($D$253,C254)</f>
+        <v>entryDrilldown.entryAcp.accessControlProfliesComboBox</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B255" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C255" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D241" s="2" t="str">
-        <f>CONCATENATE($D$239,C241)</f>
+      <c r="D255" s="2" t="str">
+        <f>CONCATENATE($D$253,C255)</f>
         <v>entryDrilldown.entryAcp.addBtn</v>
       </c>
     </row>
-    <row r="243" spans="1:7">
-      <c r="A243" s="2" t="s">
+    <row r="257" spans="1:7">
+      <c r="A257" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B243" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C243" s="2" t="s">
+      <c r="B257" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C257" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D243" s="2" t="str">
-        <f>CONCATENATE($C$221,C243)</f>
+      <c r="D257" s="2" t="str">
+        <f>CONCATENATE($C$235,C257)</f>
         <v>entryDrilldown.customData</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
-      <c r="A245" s="2" t="s">
+    <row r="259" spans="1:7">
+      <c r="A259" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B245" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C245" s="2" t="s">
+      <c r="B259" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C259" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D245" s="2" t="str">
-        <f>CONCATENATE($C$221,C245)</f>
+      <c r="D259" s="2" t="str">
+        <f>CONCATENATE($C$235,C259)</f>
         <v>entryDrilldown.entryAsstes</v>
       </c>
-      <c r="E245" s="2" t="s">
+      <c r="E259" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F245" s="2" t="s">
+      <c r="F259" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G245" s="2" t="s">
+      <c r="G259" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="247" spans="1:7">
-      <c r="A247" s="8" t="s">
+    <row r="261" spans="1:7">
+      <c r="A261" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="C261" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E247" s="2" t="s">
+      <c r="E261" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F247" s="2" t="s">
+      <c r="F261" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
-      <c r="A248" s="8" t="s">
+    <row r="262" spans="1:7">
+      <c r="A262" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="C262" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E248" s="2" t="s">
+      <c r="E262" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F248" s="2" t="s">
+      <c r="F262" s="2" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pass livestream via roles and permissions instead of flashvar
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54096 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="391">
   <si>
     <t>Dashboard</t>
   </si>
@@ -1168,6 +1168,27 @@
   </si>
   <si>
     <t>advertizingPage,contentPage</t>
+  </si>
+  <si>
+    <t>add / edit rule window</t>
+  </si>
+  <si>
+    <t>addRuleWin.</t>
+  </si>
+  <si>
+    <t>the single rule part</t>
+  </si>
+  <si>
+    <t>the filter in the rule box</t>
+  </si>
+  <si>
+    <t>singleRule.</t>
+  </si>
+  <si>
+    <t>entries</t>
+  </si>
+  <si>
+    <t>playlist entries table</t>
   </si>
 </sst>
 </file>
@@ -1553,11 +1574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G273"/>
+  <dimension ref="A1:G281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D280" sqref="D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4774,6 +4795,77 @@
       </c>
       <c r="F273" s="2" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6">
+      <c r="A277" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6">
+      <c r="A278" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D278" s="2" t="str">
+        <f>CONCATENATE($C$277,C278)</f>
+        <v>addRuleWin.saveBtn</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6">
+      <c r="A279" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D279" s="2" t="str">
+        <f>CONCATENATE($C$277,C279)</f>
+        <v>addRuleWin.singleRule.</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6">
+      <c r="A280" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D280" s="2" t="str">
+        <f>CONCATENATE($D$279,C280)</f>
+        <v>addRuleWin.singleRule.filter</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6">
+      <c r="A281" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D281" s="2" t="str">
+        <f>CONCATENATE($D$279,C281)</f>
+        <v>addRuleWin.singleRule.entries</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow ui elements on permissionGroups
git-svn-id: svn+ssh://kelev.kaltura.com/usr/local/kalsource/front/workspaces/kmc/trunk@54453 6b8eccd3-e8c5-4e7d-8186-e12b5326b719
</commit_message>
<xml_diff>
--- a/KMC/docs/components_map.xlsx
+++ b/KMC/docs/components_map.xlsx
@@ -54,15 +54,6 @@
     <t>box of account upgrade</t>
   </si>
   <si>
-    <t>dashboard.customizePanel</t>
-  </si>
-  <si>
-    <t>dashboard.chartsPanel</t>
-  </si>
-  <si>
-    <t>dashboard.accountPanel</t>
-  </si>
-  <si>
     <t>analytics</t>
   </si>
   <si>
@@ -1210,6 +1201,15 @@
   </si>
   <si>
     <t>goto content manage</t>
+  </si>
+  <si>
+    <t>chartsPanel</t>
+  </si>
+  <si>
+    <t>customizePanel</t>
+  </si>
+  <si>
+    <t>accountPanel</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1622,16 +1622,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -1653,7 +1653,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>CONCATENATE($C$2,C3)</f>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>CONCATENATE($D$3,C4)</f>
@@ -1677,13 +1677,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>CONCATENATE($D$3,C5)</f>
@@ -1698,7 +1698,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" ref="D6:D11" si="0">CONCATENATE($C$2,C6)</f>
@@ -1707,13 +1707,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>CONCATENATE($D$6,C7)</f>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>CONCATENATE($D$6,C8)</f>
@@ -1743,11 +1743,11 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>396</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dashboard.dashboard.customizePanel</v>
+        <v>dashboard.customizePanel</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1758,11 +1758,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>395</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dashboard.dashboard.chartsPanel</v>
+        <v>dashboard.chartsPanel</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1773,40 +1773,40 @@
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>397</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dashboard.dashboard.accountPanel</v>
+        <v>dashboard.accountPanel</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D21" s="2" t="str">
         <f>CONCATENATE($C$20,C21)</f>
@@ -1815,13 +1815,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D22" s="2" t="str">
         <f>CONCATENATE($C$20,C22)</f>
@@ -1830,13 +1830,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" ref="D23" si="1">CONCATENATE($C$20,C23)</f>
@@ -1845,13 +1845,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D24" s="2" t="str">
         <f>CONCATENATE($C$20,C24)</f>
@@ -1860,27 +1860,27 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>CONCATENATE($C$26,C27)</f>
@@ -1889,13 +1889,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" ref="D28:D32" si="2">CONCATENATE($C$26,C28)</f>
@@ -1904,13 +1904,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1919,13 +1919,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D31" s="2" t="str">
         <f>CONCATENATE($C$26,C31)</f>
@@ -1949,13 +1949,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1964,21 +1964,21 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D36" s="2" t="str">
         <f>CONCATENATE($C$35,C36)</f>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>CONCATENATE($C$35,C37)</f>
@@ -2002,13 +2002,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D38" s="2" t="str">
         <f>CONCATENATE($C$35,C38)</f>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" s="2" t="str">
         <f>CONCATENATE($C$35,C39)</f>
@@ -2032,27 +2032,27 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D42" s="2" t="str">
         <f t="shared" ref="D42:D63" si="3">CONCATENATE($C$41,C42)</f>
@@ -2061,13 +2061,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D43" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2076,10 +2076,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="B44" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D44" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2088,10 +2088,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="B45" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D45" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2100,13 +2100,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D46" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2115,13 +2115,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D47" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2130,13 +2130,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D48" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2145,10 +2145,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="B49" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D49" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2157,13 +2157,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D50" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2172,13 +2172,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D51" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2187,13 +2187,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D52" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="B53" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D53" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2214,10 +2214,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="B54" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D54" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="55" spans="1:4">
       <c r="B55" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D55" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2238,10 +2238,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="B56" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D56" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2250,10 +2250,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="B57" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D57" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="B58" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D58" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="B59" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D59" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2286,13 +2286,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D60" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2301,13 +2301,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D61" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2316,13 +2316,13 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D62" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2331,13 +2331,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D63" s="2" t="str">
         <f t="shared" si="3"/>
@@ -2346,21 +2346,21 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D66" s="2" t="str">
         <f>CONCATENATE($C$65,C66)</f>
@@ -2369,34 +2369,34 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D67" s="2" t="str">
         <f>CONCATENATE($C$65,C67)</f>
         <v>account.transcoding.simpleTable</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D68" s="2" t="str">
         <f>CONCATENATE($C$65,C68)</f>
@@ -2405,13 +2405,13 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D69" s="2" t="str">
         <f t="shared" ref="D69" si="4">CONCATENATE($C$65,C69)</f>
@@ -2420,13 +2420,13 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D70" s="2" t="str">
         <f t="shared" ref="D70:D74" si="5">CONCATENATE($C$65,C70)</f>
@@ -2435,13 +2435,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D71" s="2" t="str">
         <f t="shared" si="5"/>
@@ -2450,13 +2450,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D72" s="2" t="str">
         <f t="shared" si="5"/>
@@ -2465,13 +2465,13 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D73" s="2" t="str">
         <f t="shared" si="5"/>
@@ -2480,13 +2480,13 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D74" s="2" t="str">
         <f t="shared" si="5"/>
@@ -2498,24 +2498,24 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D77" s="2" t="str">
         <f>CONCATENATE($C$76,C77)</f>
@@ -2524,13 +2524,13 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D78" s="2" t="str">
         <f t="shared" ref="D78:D80" si="6">CONCATENATE($C$76,C78)</f>
@@ -2539,34 +2539,34 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D79" s="2" t="str">
         <f t="shared" si="6"/>
         <v>conversionProfileDrilldown.flavorsTable</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D80" s="2" t="str">
         <f t="shared" si="6"/>
@@ -2575,21 +2575,21 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D83" s="2" t="str">
         <f>CONCATENATE($C$82,C83)</f>
@@ -2598,13 +2598,13 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D84" s="2" t="str">
         <f>CONCATENATE($C$82,C84)</f>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D85" s="2" t="str">
         <f>CONCATENATE($C$82,C85)</f>
@@ -2628,21 +2628,21 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D88" s="2" t="str">
         <f>CONCATENATE($C$87,C88)</f>
@@ -2651,13 +2651,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D89" s="2" t="str">
         <f t="shared" ref="D89:D91" si="7">CONCATENATE($C$87,C89)</f>
@@ -2666,13 +2666,13 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D90" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2681,13 +2681,13 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D91" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2700,28 +2700,28 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D94" s="2" t="str">
         <f>CONCATENATE($C$93,C94)</f>
@@ -2731,13 +2731,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D95" s="2" t="str">
         <f t="shared" ref="D95:D101" si="8">CONCATENATE($C$93,C95)</f>
@@ -2747,13 +2747,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D96" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2764,10 +2764,10 @@
     <row r="97" spans="1:7">
       <c r="A97" s="4"/>
       <c r="B97" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D97" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2778,10 +2778,10 @@
     <row r="98" spans="1:7">
       <c r="A98" s="4"/>
       <c r="B98" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D98" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2791,13 +2791,13 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D99" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2807,13 +2807,13 @@
     </row>
     <row r="100" spans="1:7" ht="12" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D100" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2823,13 +2823,13 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D101" s="2" t="str">
         <f t="shared" si="8"/>
@@ -2838,26 +2838,26 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D105" s="2" t="str">
         <f>CONCATENATE($C$104,C105)</f>
@@ -2866,13 +2866,13 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D106" s="2" t="str">
         <f>CONCATENATE($C$104,C106)</f>
@@ -2881,13 +2881,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D107" s="2" t="str">
         <f>CONCATENATE($C$104,C107)</f>
@@ -2896,26 +2896,26 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D108" s="2" t="str">
         <f>CONCATENATE($C$104,C108)</f>
         <v>admin.users.table</v>
       </c>
       <c r="E108" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F108" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F108" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="G108" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2924,22 +2924,22 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D111" s="2" t="str">
         <f>CONCATENATE($C$110,C111)</f>
@@ -2949,10 +2949,10 @@
     <row r="112" spans="1:7">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D112" s="2" t="str">
         <f t="shared" ref="D112:D116" si="9">CONCATENATE($C$110,C112)</f>
@@ -2962,10 +2962,10 @@
     <row r="113" spans="1:7">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D113" s="2" t="str">
         <f t="shared" si="9"/>
@@ -2975,10 +2975,10 @@
     <row r="114" spans="1:7">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D114" s="2" t="str">
         <f t="shared" si="9"/>
@@ -2988,10 +2988,10 @@
     <row r="115" spans="1:7">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D115" s="2" t="str">
         <f t="shared" si="9"/>
@@ -3001,10 +3001,10 @@
     <row r="116" spans="1:7">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D116" s="2" t="str">
         <f t="shared" si="9"/>
@@ -3013,21 +3013,21 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D119" s="2" t="str">
         <f>CONCATENATE($C$118,C119)</f>
@@ -3036,13 +3036,13 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D120" s="2" t="str">
         <f t="shared" ref="D120:D122" si="10">CONCATENATE($C$118,C120)</f>
@@ -3051,13 +3051,13 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D121" s="2" t="str">
         <f t="shared" si="10"/>
@@ -3066,26 +3066,26 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D122" s="2" t="str">
         <f t="shared" si="10"/>
         <v>admin.roles.table</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3094,24 +3094,24 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D125" s="2" t="str">
         <f>CONCATENATE($C$110,C125)</f>
@@ -3120,13 +3120,13 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D126" s="2" t="str">
         <f t="shared" ref="D126:D128" si="11">CONCATENATE($C$110,C126)</f>
@@ -3135,13 +3135,13 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D127" s="2" t="str">
         <f t="shared" si="11"/>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D128" s="2" t="str">
         <f t="shared" si="11"/>
@@ -3165,35 +3165,35 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D133" s="2" t="str">
         <f>CONCATENATE($C$132,C133)</f>
@@ -3202,33 +3202,33 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D136" s="2" t="str">
         <f>CONCATENATE($C$135,C136)</f>
@@ -3237,13 +3237,13 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D138" s="1" t="str">
         <f t="shared" ref="D138" si="12">CONCATENATE($C$135,C138)</f>
@@ -3252,13 +3252,13 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D139" s="1" t="str">
         <f t="shared" ref="D139:D146" si="13">CONCATENATE($D$138,C139)</f>
@@ -3267,13 +3267,13 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D140" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3282,13 +3282,13 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D141" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3297,13 +3297,13 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D142" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3312,13 +3312,13 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D143" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3327,13 +3327,13 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D144" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D145" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3357,13 +3357,13 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D146" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3372,34 +3372,34 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D148" s="2" t="str">
         <f>CONCATENATE($C$135,C148)</f>
         <v>wizard.featurePage.</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D149" s="2" t="str">
         <f>CONCATENATE($D$148,C149)</f>
@@ -3408,13 +3408,13 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D150" s="2" t="str">
         <f>CONCATENATE($D$148,C150)</f>
@@ -3423,13 +3423,13 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D151" s="2" t="str">
         <f>CONCATENATE($D$148,C151)</f>
@@ -3438,13 +3438,13 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D153" s="2" t="str">
         <f>CONCATENATE($C$135,C153)</f>
@@ -3453,13 +3453,13 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D155" s="2" t="str">
         <f>CONCATENATE($C$135,C155)</f>
@@ -3468,13 +3468,13 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D157" s="2" t="str">
         <f>CONCATENATE($C$135,C157)</f>
@@ -3483,13 +3483,13 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D158" s="2" t="str">
         <f>CONCATENATE($D$157,C158)</f>
@@ -3498,13 +3498,13 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D160" s="2" t="str">
         <f>CONCATENATE($C$135,C160)</f>
@@ -3513,13 +3513,13 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D161" s="2" t="str">
         <f t="shared" ref="D161:D166" si="14">CONCATENATE($D$160,C161)</f>
@@ -3528,13 +3528,13 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D162" s="2" t="str">
         <f t="shared" si="14"/>
@@ -3543,13 +3543,13 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D163" s="2" t="str">
         <f t="shared" si="14"/>
@@ -3558,13 +3558,13 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D164" s="2" t="str">
         <f t="shared" si="14"/>
@@ -3573,13 +3573,13 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D165" s="2" t="str">
         <f t="shared" si="14"/>
@@ -3588,13 +3588,13 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D166" s="2" t="str">
         <f t="shared" si="14"/>
@@ -3603,40 +3603,40 @@
     </row>
     <row r="170" spans="1:6">
       <c r="A170" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D173" s="2" t="str">
         <f>CONCATENATE($C$172,C173)</f>
@@ -3645,34 +3645,34 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D175" s="2" t="str">
         <f>CONCATENATE($C$172,C175)</f>
         <v>content.manage.toolBar.</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D176" s="2" t="str">
         <f>CONCATENATE($D$175,C176)</f>
@@ -3681,13 +3681,13 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D177" s="2" t="str">
         <f t="shared" ref="D177:D181" si="15">CONCATENATE($D$175,C177)</f>
@@ -3696,13 +3696,13 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D178" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3711,13 +3711,13 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D179" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3726,13 +3726,13 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D180" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3741,13 +3741,13 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D181" s="2" t="str">
         <f t="shared" si="15"/>
@@ -3756,34 +3756,34 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C183" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D183" s="2" t="str">
         <f>CONCATENATE($C$172,C183)</f>
         <v>content.manage.filter.</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D184" s="2" t="str">
         <f>CONCATENATE($D$183,C184)</f>
@@ -3792,13 +3792,13 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D185" s="2" t="str">
         <f t="shared" ref="D185:D193" si="16">CONCATENATE($D$183,C185)</f>
@@ -3807,13 +3807,13 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D186" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3822,13 +3822,13 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D187" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3837,13 +3837,13 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D188" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D189" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3867,13 +3867,13 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D190" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3882,13 +3882,13 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D191" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3897,13 +3897,13 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D192" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3912,13 +3912,13 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D193" s="2" t="str">
         <f t="shared" si="16"/>
@@ -3927,42 +3927,42 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="196" spans="1:6">
       <c r="A196" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C196" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D196" s="2" t="str">
         <f>CONCATENATE($C$195,C196)</f>
         <v>content.moderation.filter.</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D197" s="2" t="str">
         <f>CONCATENATE($D$183,C197)</f>
@@ -3971,13 +3971,13 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D198" s="2" t="str">
         <f t="shared" ref="D198:D206" si="17">CONCATENATE($D$183,C198)</f>
@@ -3986,13 +3986,13 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D199" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4001,13 +4001,13 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D200" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4016,13 +4016,13 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D201" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4031,13 +4031,13 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D202" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4046,13 +4046,13 @@
     </row>
     <row r="203" spans="1:6">
       <c r="A203" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D203" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4061,13 +4061,13 @@
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D204" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4076,13 +4076,13 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D205" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4091,13 +4091,13 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D206" s="2" t="str">
         <f t="shared" si="17"/>
@@ -4106,13 +4106,13 @@
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D208" s="2" t="str">
         <f>CONCATENATE($C$195,C208)</f>
@@ -4121,13 +4121,13 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D209" s="2" t="str">
         <f>CONCATENATE($C$195,C209)</f>
@@ -4136,13 +4136,13 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D210" s="2" t="str">
         <f>CONCATENATE($D$209,C210)</f>
@@ -4151,13 +4151,13 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D211" s="2" t="str">
         <f>CONCATENATE($D$209,C211)</f>
@@ -4166,21 +4166,21 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D214" s="2" t="str">
         <f>CONCATENATE($C$213,C214)</f>
@@ -4189,13 +4189,13 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D215" s="2" t="str">
         <f>CONCATENATE($D$214,C215)</f>
@@ -4204,13 +4204,13 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D216" s="2" t="str">
         <f>CONCATENATE($D$214,C216)</f>
@@ -4219,13 +4219,13 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D218" s="2" t="str">
         <f t="shared" ref="D218:D224" si="18">CONCATENATE($C$213,C218)</f>
@@ -4234,13 +4234,13 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D219" s="2" t="str">
         <f t="shared" si="18"/>
@@ -4249,13 +4249,13 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D220" s="2" t="str">
         <f>CONCATENATE($D$219,C220)</f>
@@ -4264,13 +4264,13 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D222" s="2" t="str">
         <f t="shared" si="18"/>
@@ -4279,13 +4279,13 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D223" s="2" t="str">
         <f t="shared" si="18"/>
@@ -4294,13 +4294,13 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D224" s="2" t="str">
         <f t="shared" si="18"/>
@@ -4309,21 +4309,21 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D227" s="2" t="str">
         <f>CONCATENATE($C$226,C227)</f>
@@ -4332,13 +4332,13 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D228" s="2" t="str">
         <f>CONCATENATE($C$226,C228)</f>
@@ -4347,13 +4347,13 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D229" s="2" t="str">
         <f t="shared" ref="D229:D230" si="19">CONCATENATE($C$226,C229)</f>
@@ -4362,13 +4362,13 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D230" s="2" t="str">
         <f t="shared" si="19"/>
@@ -4377,32 +4377,32 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C232" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E232" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E232" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F232" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D235" s="2" t="str">
         <f>CONCATENATE($C$234,C235)</f>
@@ -4411,13 +4411,13 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D236" s="2" t="str">
         <f t="shared" ref="D236:D237" si="20">CONCATENATE($C$234,C236)</f>
@@ -4426,13 +4426,13 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D237" s="2" t="str">
         <f t="shared" si="20"/>
@@ -4441,10 +4441,10 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D238" s="2" t="str">
         <f t="shared" ref="D238:D239" si="21">CONCATENATE($C$234,C238)</f>
@@ -4453,13 +4453,13 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D239" s="2" t="str">
         <f t="shared" si="21"/>
@@ -4468,51 +4468,51 @@
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G241" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="242" spans="1:7">
       <c r="A242" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D242" s="2" t="str">
         <f>CONCATENATE($C$241,C242)</f>
         <v>entryDrilldown.entryMetaData.</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F242" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D243" s="2" t="str">
         <f>CONCATENATE($D$242,C243)</f>
@@ -4521,13 +4521,13 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D244" s="2" t="str">
         <f>CONCATENATE($D$242,C244)</f>
@@ -4536,13 +4536,13 @@
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D245" s="2" t="str">
         <f>CONCATENATE($D$242,C245)</f>
@@ -4551,13 +4551,13 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D246" s="2" t="str">
         <f>CONCATENATE($D$242,C246)</f>
@@ -4566,13 +4566,13 @@
     </row>
     <row r="247" spans="1:7">
       <c r="A247" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D247" s="2" t="str">
         <f>CONCATENATE($D$242,C247)</f>
@@ -4581,34 +4581,34 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B252" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D252" s="2" t="str">
         <f>CONCATENATE($C$241,C252)</f>
         <v>entryDrilldown.entrySch.</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F252" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G252" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="253" spans="1:7">
       <c r="B253" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D253" s="2" t="str">
         <f>CONCATENATE($D$252,C253)</f>
@@ -4617,10 +4617,10 @@
     </row>
     <row r="254" spans="1:7">
       <c r="B254" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D254" s="2" t="str">
         <f t="shared" ref="D254:D260" si="22">CONCATENATE($D$252,C254)</f>
@@ -4629,10 +4629,10 @@
     </row>
     <row r="255" spans="1:7">
       <c r="B255" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D255" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4641,10 +4641,10 @@
     </row>
     <row r="256" spans="1:7">
       <c r="B256" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D256" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4653,10 +4653,10 @@
     </row>
     <row r="257" spans="1:4">
       <c r="B257" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D257" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4665,10 +4665,10 @@
     </row>
     <row r="258" spans="1:4">
       <c r="B258" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C258" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="D258" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4677,10 +4677,10 @@
     </row>
     <row r="259" spans="1:4">
       <c r="B259" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D259" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4689,10 +4689,10 @@
     </row>
     <row r="260" spans="1:4">
       <c r="B260" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D260" s="2" t="str">
         <f t="shared" si="22"/>
@@ -4701,13 +4701,13 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D262" s="2" t="str">
         <f>CONCATENATE($C$241,C262)</f>
@@ -4716,13 +4716,13 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D263" s="2" t="str">
         <f>CONCATENATE($D$262,C263)</f>
@@ -4731,13 +4731,13 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D264" s="2" t="str">
         <f>CONCATENATE($D$262,C264)</f>
@@ -4746,13 +4746,13 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" s="4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B266" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D266" s="2" t="str">
         <f>CONCATENATE($C$241,C266)</f>
@@ -4765,7 +4765,7 @@
         <v>6</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D267" s="2" t="str">
         <f>CONCATENATE($D$266,C267)</f>
@@ -4777,7 +4777,7 @@
         <v>6</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D268" s="2" t="str">
         <f>CONCATENATE($D$266,C268)</f>
@@ -4789,7 +4789,7 @@
         <v>6</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D269" s="2" t="str">
         <f>CONCATENATE($D$266,C269)</f>
@@ -4798,13 +4798,13 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D270" s="2" t="str">
         <f>CONCATENATE($D$266,C270)</f>
@@ -4813,13 +4813,13 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D272" s="2" t="str">
         <f>CONCATENATE($C$241,C272)</f>
@@ -4828,76 +4828,76 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D274" s="2" t="str">
         <f>CONCATENATE($C$241,C274)</f>
         <v>entryDrilldown.entryAsstes</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F274" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G274" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="281" spans="1:7">
       <c r="A281" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="282" spans="1:7">
       <c r="A282" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D282" s="2" t="str">
         <f>CONCATENATE($C$281,C282)</f>
@@ -4906,13 +4906,13 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D283" s="2" t="str">
         <f>CONCATENATE($C$281,C283)</f>
@@ -4921,13 +4921,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D284" s="2" t="str">
         <f>CONCATENATE($D$283,C284)</f>
@@ -4936,13 +4936,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D285" s="2" t="str">
         <f>CONCATENATE($D$283,C285)</f>

</xml_diff>